<commit_message>
final + cleanup and sort
</commit_message>
<xml_diff>
--- a/weedDepthTake3.xlsx
+++ b/weedDepthTake3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EC7"/>
+  <dimension ref="A1:EU7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -833,215 +833,287 @@
       <c r="EC1" s="1" t="n">
         <v>132</v>
       </c>
+      <c r="ED1" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="EE1" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="EF1" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="EG1" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="EH1" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="EI1" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="EJ1" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="EK1" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="EL1" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="EM1" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="EN1" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="EO1" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="EP1" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="EQ1" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="ER1" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="ES1" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="ET1" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="EU1" s="1" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.3739907741546631</v>
+        <v>-0.0672764927148819</v>
       </c>
       <c r="B2" t="n">
-        <v>0.373988151550293</v>
+        <v>-0.06727827340364456</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3739892840385437</v>
+        <v>-0.06727313995361328</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3739885091781616</v>
+        <v>-0.06727314740419388</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3739895820617676</v>
+        <v>-0.06727760285139084</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3739886283874512</v>
+        <v>-0.06727225333452225</v>
       </c>
       <c r="G2" t="n">
-        <v>0.373990386724472</v>
+        <v>-0.06727474927902222</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3739905953407288</v>
+        <v>-0.06727492064237595</v>
       </c>
       <c r="I2" t="n">
-        <v>0.373988002538681</v>
+        <v>-0.0672793835401535</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3739870190620422</v>
+        <v>-0.06727046519517899</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3739899396896362</v>
+        <v>-0.06726868450641632</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3739888072013855</v>
+        <v>-0.06727582216262817</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3739892244338989</v>
+        <v>-0.06728094816207886</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3739901185035706</v>
+        <v>-0.0672764927148819</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3739888072013855</v>
+        <v>-0.06727582216262817</v>
       </c>
       <c r="P2" t="n">
-        <v>0.373990535736084</v>
+        <v>-0.06727413833141327</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.3739905953407288</v>
+        <v>-0.06727314740419388</v>
       </c>
       <c r="R2" t="n">
-        <v>0.3739897608757019</v>
+        <v>-0.06727313995361328</v>
       </c>
       <c r="S2" t="n">
-        <v>0.373988151550293</v>
+        <v>-0.06727760285139084</v>
       </c>
       <c r="T2" t="n">
-        <v>0.373991847038269</v>
+        <v>-0.06728184223175049</v>
       </c>
       <c r="U2" t="n">
-        <v>0.3739889860153198</v>
+        <v>-0.06727564334869385</v>
       </c>
       <c r="V2" t="n">
-        <v>0.3739897608757019</v>
+        <v>-0.06727760285139084</v>
       </c>
       <c r="W2" t="n">
-        <v>0.3739906549453735</v>
+        <v>-0.06727848947048187</v>
       </c>
       <c r="X2" t="n">
-        <v>0.3739893436431885</v>
+        <v>-0.06727307289838791</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.3739874362945557</v>
+        <v>-0.06727580726146698</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.3739885091781616</v>
+        <v>-0.0672764927148819</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.3739897012710571</v>
+        <v>-0.06727670878171921</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.3739883899688721</v>
+        <v>-0.06727916747331619</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.373989462852478</v>
+        <v>-0.06727564334869385</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.3739775121212006</v>
+        <v>-0.06727759540081024</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.3738406300544739</v>
+        <v>-0.06727207452058792</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.3741002678871155</v>
+        <v>-0.06727474927902222</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.3739690482616425</v>
+        <v>-0.06727564334869385</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.373996376991272</v>
+        <v>-0.06726551055908203</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.3737013041973114</v>
+        <v>-0.06518979370594025</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.3734043538570404</v>
+        <v>-0.0625062957406044</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.3732696771621704</v>
+        <v>-0.06142423674464226</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.3730896711349487</v>
+        <v>-0.05851275473833084</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.3728930354118347</v>
+        <v>-0.0563330166041851</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.3727510571479797</v>
+        <v>-0.05344094336032867</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.372475802898407</v>
+        <v>-0.05145208165049553</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.3725394606590271</v>
+        <v>-0.04987892135977745</v>
       </c>
       <c r="AQ2" t="n">
-        <v>0.37716144323349</v>
+        <v>-0.04868118092417717</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.3833906054496765</v>
+        <v>-0.04694539308547974</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.3897520899772644</v>
+        <v>-0.04474370554089546</v>
       </c>
       <c r="AT2" t="n">
-        <v>0.3962013721466064</v>
+        <v>-0.04258942231535912</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.4024225473403931</v>
+        <v>-0.04029867425560951</v>
       </c>
       <c r="AV2" t="n">
-        <v>0.4101806282997131</v>
+        <v>-0.03770944476127625</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.4164556860923767</v>
+        <v>-0.03614207729697227</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.4241616725921631</v>
+        <v>-0.03492633625864983</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.4303284287452698</v>
+        <v>-0.03428634256124496</v>
       </c>
       <c r="AZ2" t="n">
-        <v>0.4365720450878143</v>
+        <v>-0.03292278200387955</v>
       </c>
       <c r="BA2" t="n">
-        <v>0.4428946673870087</v>
+        <v>-0.03226296603679657</v>
       </c>
       <c r="BB2" t="n">
-        <v>0.4492589235305786</v>
+        <v>-0.03195701912045479</v>
       </c>
       <c r="BC2" t="n">
-        <v>0.4554064273834229</v>
+        <v>-0.03162122517824173</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.4616508781909943</v>
+        <v>-0.0312182791531086</v>
       </c>
       <c r="BE2" t="n">
-        <v>0.4691238105297089</v>
+        <v>-0.03113839030265808</v>
       </c>
       <c r="BF2" t="n">
-        <v>0.4755396842956543</v>
+        <v>-0.0301157683134079</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.4817160964012146</v>
+        <v>-0.02959166839718819</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.4879331588745117</v>
+        <v>-0.029451048001647</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.4941795468330383</v>
+        <v>-0.02966141887009144</v>
       </c>
       <c r="BJ2" t="n">
-        <v>0.5002967715263367</v>
+        <v>-0.02998756244778633</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.5065296292304993</v>
+        <v>-0.03002091869711876</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.5128663778305054</v>
+        <v>-0.03003714606165886</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.519107460975647</v>
+        <v>-0.03010239824652672</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.5252457857131958</v>
-      </c>
-      <c r="BO2" t="inlineStr"/>
-      <c r="BP2" t="inlineStr"/>
-      <c r="BQ2" t="inlineStr"/>
-      <c r="BR2" t="inlineStr"/>
-      <c r="BS2" t="inlineStr"/>
-      <c r="BT2" t="inlineStr"/>
-      <c r="BU2" t="inlineStr"/>
-      <c r="BV2" t="inlineStr"/>
-      <c r="BW2" t="inlineStr"/>
+        <v>-0.02857845276594162</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>-0.02759779989719391</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>-0.02669366076588631</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>-0.02627201750874519</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>-0.02549014985561371</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>-0.0251185167580843</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>-0.0251725111156702</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>-0.02493898198008537</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>-0.02449499070644379</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>-0.0234505906701088</v>
+      </c>
       <c r="BX2" t="inlineStr"/>
       <c r="BY2" t="inlineStr"/>
       <c r="BZ2" t="inlineStr"/>
@@ -1100,215 +1172,251 @@
       <c r="EA2" t="inlineStr"/>
       <c r="EB2" t="inlineStr"/>
       <c r="EC2" t="inlineStr"/>
+      <c r="ED2" t="inlineStr"/>
+      <c r="EE2" t="inlineStr"/>
+      <c r="EF2" t="inlineStr"/>
+      <c r="EG2" t="inlineStr"/>
+      <c r="EH2" t="inlineStr"/>
+      <c r="EI2" t="inlineStr"/>
+      <c r="EJ2" t="inlineStr"/>
+      <c r="EK2" t="inlineStr"/>
+      <c r="EL2" t="inlineStr"/>
+      <c r="EM2" t="inlineStr"/>
+      <c r="EN2" t="inlineStr"/>
+      <c r="EO2" t="inlineStr"/>
+      <c r="EP2" t="inlineStr"/>
+      <c r="EQ2" t="inlineStr"/>
+      <c r="ER2" t="inlineStr"/>
+      <c r="ES2" t="inlineStr"/>
+      <c r="ET2" t="inlineStr"/>
+      <c r="EU2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.2518103122711182</v>
+        <v>258</v>
       </c>
       <c r="B3" t="n">
-        <v>0.251812070608139</v>
+        <v>258</v>
       </c>
       <c r="C3" t="n">
-        <v>0.251810759305954</v>
+        <v>258</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2518087923526764</v>
+        <v>258</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2518115639686584</v>
+        <v>258</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2518123984336853</v>
+        <v>258</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2518141269683838</v>
+        <v>258</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2518115639686584</v>
+        <v>258</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2518100738525391</v>
+        <v>258</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2518104910850525</v>
+        <v>258</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2518148124217987</v>
+        <v>258</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2518098950386047</v>
+        <v>258</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2518101036548615</v>
+        <v>258</v>
       </c>
       <c r="N3" t="n">
-        <v>0.251812756061554</v>
+        <v>258</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2518091797828674</v>
+        <v>258</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2518145442008972</v>
+        <v>258</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.2518104910850525</v>
+        <v>259</v>
       </c>
       <c r="R3" t="n">
-        <v>0.251806914806366</v>
+        <v>258</v>
       </c>
       <c r="S3" t="n">
-        <v>0.2518133223056793</v>
+        <v>259</v>
       </c>
       <c r="T3" t="n">
-        <v>0.2518130540847778</v>
+        <v>259</v>
       </c>
       <c r="U3" t="n">
-        <v>0.2518092393875122</v>
+        <v>258</v>
       </c>
       <c r="V3" t="n">
-        <v>0.2518143057823181</v>
+        <v>258</v>
       </c>
       <c r="W3" t="n">
-        <v>0.2518126368522644</v>
+        <v>258</v>
       </c>
       <c r="X3" t="n">
-        <v>0.2518123686313629</v>
+        <v>258</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.251809149980545</v>
+        <v>258</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.2518117427825928</v>
+        <v>258</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.251811683177948</v>
+        <v>258</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.2518120408058167</v>
+        <v>258</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.2518112659454346</v>
+        <v>259</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.2518214285373688</v>
+        <v>258</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.2543957233428955</v>
+        <v>258</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.2572372257709503</v>
+        <v>258</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.2603128850460052</v>
+        <v>259</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.2626411318778992</v>
+        <v>258</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.2652548849582672</v>
+        <v>259</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.2672698497772217</v>
+        <v>257</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.2695773243904114</v>
+        <v>248</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.2721223831176758</v>
+        <v>244</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.2743492424488068</v>
+        <v>241</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.2769801318645477</v>
+        <v>238</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.2789070606231689</v>
+        <v>233</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.2803808152675629</v>
+        <v>230</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.2825205326080322</v>
+        <v>228</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.2850668132305145</v>
+        <v>225</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.2857896685600281</v>
+        <v>228</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.2868750989437103</v>
+        <v>220</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.2871126532554626</v>
+        <v>216</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.2873017489910126</v>
+        <v>209</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.2869164645671844</v>
+        <v>210</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.2866031229496002</v>
+        <v>204</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.2856910228729248</v>
+        <v>201</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.2846938073635101</v>
+        <v>199</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.2842879891395569</v>
+        <v>197</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.2841883897781372</v>
+        <v>197</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.2840054929256439</v>
+        <v>192</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.2837056219577789</v>
+        <v>190</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.2835323512554169</v>
+        <v>191</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.2839025259017944</v>
+        <v>182</v>
       </c>
       <c r="BG3" t="n">
-        <v>0.2846264243125916</v>
+        <v>174</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.2850891947746277</v>
+        <v>172</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.2853519320487976</v>
+        <v>172</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.2852025628089905</v>
+        <v>172</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.285735547542572</v>
+        <v>171</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.2863963842391968</v>
+        <v>172</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.2866148352622986</v>
+        <v>170</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.2872598171234131</v>
-      </c>
-      <c r="BO3" t="inlineStr"/>
-      <c r="BP3" t="inlineStr"/>
-      <c r="BQ3" t="inlineStr"/>
-      <c r="BR3" t="inlineStr"/>
-      <c r="BS3" t="inlineStr"/>
-      <c r="BT3" t="inlineStr"/>
-      <c r="BU3" t="inlineStr"/>
-      <c r="BV3" t="inlineStr"/>
-      <c r="BW3" t="inlineStr"/>
+        <v>168</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>169</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>166</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>166</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>165</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>166</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>167</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>166</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>165</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>163</v>
+      </c>
       <c r="BX3" t="inlineStr"/>
       <c r="BY3" t="inlineStr"/>
       <c r="BZ3" t="inlineStr"/>
@@ -1367,616 +1475,554 @@
       <c r="EA3" t="inlineStr"/>
       <c r="EB3" t="inlineStr"/>
       <c r="EC3" t="inlineStr"/>
+      <c r="ED3" t="inlineStr"/>
+      <c r="EE3" t="inlineStr"/>
+      <c r="EF3" t="inlineStr"/>
+      <c r="EG3" t="inlineStr"/>
+      <c r="EH3" t="inlineStr"/>
+      <c r="EI3" t="inlineStr"/>
+      <c r="EJ3" t="inlineStr"/>
+      <c r="EK3" t="inlineStr"/>
+      <c r="EL3" t="inlineStr"/>
+      <c r="EM3" t="inlineStr"/>
+      <c r="EN3" t="inlineStr"/>
+      <c r="EO3" t="inlineStr"/>
+      <c r="EP3" t="inlineStr"/>
+      <c r="EQ3" t="inlineStr"/>
+      <c r="ER3" t="inlineStr"/>
+      <c r="ES3" t="inlineStr"/>
+      <c r="ET3" t="inlineStr"/>
+      <c r="EU3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15820240900</v>
+        <v>0.2518490850925446</v>
       </c>
       <c r="B4" t="n">
-        <v>15820240900</v>
+        <v>0.2518492043018341</v>
       </c>
       <c r="C4" t="n">
-        <v>16062180200</v>
+        <v>0.2518498003482819</v>
       </c>
       <c r="D4" t="n">
-        <v>16062180200</v>
+        <v>0.2518519163131714</v>
       </c>
       <c r="E4" t="n">
-        <v>16163595100</v>
+        <v>0.2518483698368073</v>
       </c>
       <c r="F4" t="n">
-        <v>16163595100</v>
+        <v>0.2518510520458221</v>
       </c>
       <c r="G4" t="n">
-        <v>16286693600</v>
+        <v>0.2518507242202759</v>
       </c>
       <c r="H4" t="n">
-        <v>16286693600</v>
+        <v>0.2518466711044312</v>
       </c>
       <c r="I4" t="n">
-        <v>16413562300</v>
+        <v>0.2518490254878998</v>
       </c>
       <c r="J4" t="n">
-        <v>16413562300</v>
+        <v>0.251846581697464</v>
       </c>
       <c r="K4" t="n">
-        <v>16510386400</v>
+        <v>0.2518476247787476</v>
       </c>
       <c r="L4" t="n">
-        <v>16510386400</v>
+        <v>0.2518509924411774</v>
       </c>
       <c r="M4" t="n">
-        <v>16613914300</v>
+        <v>0.2518505752086639</v>
       </c>
       <c r="N4" t="n">
-        <v>16613914300</v>
+        <v>0.2518472671508789</v>
       </c>
       <c r="O4" t="n">
-        <v>16738824100</v>
+        <v>0.251848578453064</v>
       </c>
       <c r="P4" t="n">
-        <v>16738824100</v>
+        <v>0.2518452703952789</v>
       </c>
       <c r="Q4" t="n">
-        <v>16861427400</v>
+        <v>0.2518473565578461</v>
       </c>
       <c r="R4" t="n">
-        <v>16861427400</v>
+        <v>0.2518517374992371</v>
       </c>
       <c r="S4" t="n">
-        <v>16986648800</v>
+        <v>0.2518488466739655</v>
       </c>
       <c r="T4" t="n">
-        <v>16986648800</v>
+        <v>0.2518502771854401</v>
       </c>
       <c r="U4" t="n">
-        <v>17111483300</v>
+        <v>0.2518540322780609</v>
       </c>
       <c r="V4" t="n">
-        <v>17111483300</v>
+        <v>0.2518505156040192</v>
       </c>
       <c r="W4" t="n">
-        <v>17237742100</v>
+        <v>0.2518478333950043</v>
       </c>
       <c r="X4" t="n">
-        <v>17237742100</v>
+        <v>0.2518524825572968</v>
       </c>
       <c r="Y4" t="n">
-        <v>17338520800</v>
+        <v>0.2518487572669983</v>
       </c>
       <c r="Z4" t="n">
-        <v>17338520800</v>
+        <v>0.251849353313446</v>
       </c>
       <c r="AA4" t="n">
-        <v>17463846100</v>
+        <v>0.2518483400344849</v>
       </c>
       <c r="AB4" t="n">
-        <v>17463846100</v>
+        <v>0.2518493831157684</v>
       </c>
       <c r="AC4" t="n">
-        <v>17588828200</v>
+        <v>0.2518513798713684</v>
       </c>
       <c r="AD4" t="n">
-        <v>17588828200</v>
+        <v>0.2518508434295654</v>
       </c>
       <c r="AE4" t="n">
-        <v>17721630500</v>
+        <v>0.2518494427204132</v>
       </c>
       <c r="AF4" t="n">
-        <v>17721630500</v>
+        <v>0.2518534362316132</v>
       </c>
       <c r="AG4" t="n">
-        <v>17873507900</v>
+        <v>0.2518503367900848</v>
       </c>
       <c r="AH4" t="n">
-        <v>17873507900</v>
+        <v>0.2518687546253204</v>
       </c>
       <c r="AI4" t="n">
-        <v>18017089300</v>
+        <v>0.2506610453128815</v>
       </c>
       <c r="AJ4" t="n">
-        <v>18017089300</v>
+        <v>0.2473911494016647</v>
       </c>
       <c r="AK4" t="n">
-        <v>18138692000</v>
+        <v>0.2456622719764709</v>
       </c>
       <c r="AL4" t="n">
-        <v>18138692000</v>
+        <v>0.2428667396306992</v>
       </c>
       <c r="AM4" t="n">
-        <v>18266755200</v>
+        <v>0.240818589925766</v>
       </c>
       <c r="AN4" t="n">
-        <v>18266755200</v>
+        <v>0.2385523617267609</v>
       </c>
       <c r="AO4" t="n">
-        <v>18390182200</v>
+        <v>0.2366505563259125</v>
       </c>
       <c r="AP4" t="n">
-        <v>18390182200</v>
+        <v>0.2350364923477173</v>
       </c>
       <c r="AQ4" t="n">
-        <v>18526466400</v>
+        <v>0.2332315891981125</v>
       </c>
       <c r="AR4" t="n">
-        <v>18526466400</v>
+        <v>0.2316875606775284</v>
       </c>
       <c r="AS4" t="n">
-        <v>18642066700</v>
+        <v>0.2294118404388428</v>
       </c>
       <c r="AT4" t="n">
-        <v>18642066700</v>
+        <v>0.2275154888629913</v>
       </c>
       <c r="AU4" t="n">
-        <v>18766918400</v>
+        <v>0.2250328361988068</v>
       </c>
       <c r="AV4" t="n">
-        <v>18766918400</v>
+        <v>0.2231327444314957</v>
       </c>
       <c r="AW4" t="n">
-        <v>18893062400</v>
+        <v>0.2217909246683121</v>
       </c>
       <c r="AX4" t="n">
-        <v>18893062400</v>
+        <v>0.2200163602828979</v>
       </c>
       <c r="AY4" t="n">
-        <v>19013168800</v>
+        <v>0.2184580415487289</v>
       </c>
       <c r="AZ4" t="n">
-        <v>19013168800</v>
+        <v>0.2161207944154739</v>
       </c>
       <c r="BA4" t="n">
-        <v>19140788600</v>
+        <v>0.2143111526966095</v>
       </c>
       <c r="BB4" t="n">
-        <v>19140788600</v>
+        <v>0.2132555842399597</v>
       </c>
       <c r="BC4" t="n">
-        <v>19266309700</v>
+        <v>0.2115977257490158</v>
       </c>
       <c r="BD4" t="n">
-        <v>19266309700</v>
+        <v>0.2106547504663467</v>
       </c>
       <c r="BE4" t="n">
-        <v>19385341100</v>
+        <v>0.2092414796352386</v>
       </c>
       <c r="BF4" t="n">
-        <v>19385341100</v>
+        <v>0.2067586034536362</v>
       </c>
       <c r="BG4" t="n">
-        <v>19524599500</v>
+        <v>0.2042021900415421</v>
       </c>
       <c r="BH4" t="n">
-        <v>19524599500</v>
+        <v>0.2029288858175278</v>
       </c>
       <c r="BI4" t="n">
-        <v>19654413400</v>
+        <v>0.2020822763442993</v>
       </c>
       <c r="BJ4" t="n">
-        <v>19654413400</v>
+        <v>0.2012858092784882</v>
       </c>
       <c r="BK4" t="n">
-        <v>19798754400</v>
+        <v>0.1997993439435959</v>
       </c>
       <c r="BL4" t="n">
-        <v>19798754400</v>
+        <v>0.1989577561616898</v>
       </c>
       <c r="BM4" t="n">
-        <v>19924905100</v>
+        <v>0.1981549561023712</v>
       </c>
       <c r="BN4" t="n">
-        <v>19924905100</v>
+        <v>0.1966294199228287</v>
       </c>
       <c r="BO4" t="n">
-        <v>20073202700</v>
+        <v>0.196053609251976</v>
       </c>
       <c r="BP4" t="n">
-        <v>20073202700</v>
+        <v>0.1952443271875381</v>
       </c>
       <c r="BQ4" t="n">
-        <v>20206831100</v>
+        <v>0.1943223029375076</v>
       </c>
       <c r="BR4" t="n">
-        <v>20206831100</v>
+        <v>0.1934070438146591</v>
       </c>
       <c r="BS4" t="n">
-        <v>20328967200</v>
+        <v>0.1927557736635208</v>
       </c>
       <c r="BT4" t="n">
-        <v>20328967200</v>
+        <v>0.1922584176063538</v>
       </c>
       <c r="BU4" t="n">
-        <v>20449082400</v>
+        <v>0.1916122436523438</v>
       </c>
       <c r="BV4" t="n">
-        <v>20449082400</v>
+        <v>0.1909289360046387</v>
       </c>
       <c r="BW4" t="n">
-        <v>20573747900</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>20573747900</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>20698870300</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>20698870300</v>
-      </c>
-      <c r="CA4" t="n">
-        <v>20824464900</v>
-      </c>
-      <c r="CB4" t="n">
-        <v>20824464900</v>
-      </c>
-      <c r="CC4" t="n">
-        <v>20951440200</v>
-      </c>
-      <c r="CD4" t="n">
-        <v>20951440200</v>
-      </c>
-      <c r="CE4" t="n">
-        <v>21076843400</v>
-      </c>
-      <c r="CF4" t="n">
-        <v>21076843400</v>
-      </c>
-      <c r="CG4" t="n">
-        <v>21202879900</v>
-      </c>
-      <c r="CH4" t="n">
-        <v>21202879900</v>
-      </c>
-      <c r="CI4" t="n">
-        <v>21323914700</v>
-      </c>
-      <c r="CJ4" t="n">
-        <v>21323914700</v>
-      </c>
-      <c r="CK4" t="n">
-        <v>21450706100</v>
-      </c>
-      <c r="CL4" t="n">
-        <v>21450706100</v>
-      </c>
-      <c r="CM4" t="n">
-        <v>21576350500</v>
-      </c>
-      <c r="CN4" t="n">
-        <v>21576350500</v>
-      </c>
-      <c r="CO4" t="n">
-        <v>21700453300</v>
-      </c>
-      <c r="CP4" t="n">
-        <v>21700453300</v>
-      </c>
-      <c r="CQ4" t="n">
-        <v>21824748600</v>
-      </c>
-      <c r="CR4" t="n">
-        <v>21824748600</v>
-      </c>
-      <c r="CS4" t="n">
-        <v>21973043700</v>
-      </c>
-      <c r="CT4" t="n">
-        <v>21973043700</v>
-      </c>
-      <c r="CU4" t="n">
-        <v>22098961700</v>
-      </c>
-      <c r="CV4" t="n">
-        <v>22098961700</v>
-      </c>
-      <c r="CW4" t="n">
-        <v>22252302100</v>
-      </c>
-      <c r="CX4" t="n">
-        <v>22252302100</v>
-      </c>
-      <c r="CY4" t="n">
-        <v>22376396900</v>
-      </c>
-      <c r="CZ4" t="n">
-        <v>22376396900</v>
-      </c>
-      <c r="DA4" t="n">
-        <v>22501698800</v>
-      </c>
-      <c r="DB4" t="n">
-        <v>22501698800</v>
-      </c>
-      <c r="DC4" t="n">
-        <v>22625739300</v>
-      </c>
-      <c r="DD4" t="n">
-        <v>22625739300</v>
-      </c>
-      <c r="DE4" t="n">
-        <v>22748854400</v>
-      </c>
-      <c r="DF4" t="n">
-        <v>22748854400</v>
-      </c>
-      <c r="DG4" t="n">
-        <v>22876286000</v>
-      </c>
-      <c r="DH4" t="n">
-        <v>22876286000</v>
-      </c>
-      <c r="DI4" t="n">
-        <v>23029098100</v>
-      </c>
-      <c r="DJ4" t="n">
-        <v>23029098100</v>
-      </c>
-      <c r="DK4" t="n">
-        <v>23149928200</v>
-      </c>
-      <c r="DL4" t="n">
-        <v>23149928200</v>
-      </c>
-      <c r="DM4" t="n">
-        <v>23273279600</v>
-      </c>
-      <c r="DN4" t="n">
-        <v>23273279600</v>
-      </c>
-      <c r="DO4" t="n">
-        <v>23398622200</v>
-      </c>
-      <c r="DP4" t="n">
-        <v>23398622200</v>
-      </c>
-      <c r="DQ4" t="n">
-        <v>23524886500</v>
-      </c>
-      <c r="DR4" t="n">
-        <v>23524886500</v>
-      </c>
-      <c r="DS4" t="n">
-        <v>23649267300</v>
-      </c>
-      <c r="DT4" t="n">
-        <v>23649267300</v>
-      </c>
-      <c r="DU4" t="n">
-        <v>23774414400</v>
-      </c>
-      <c r="DV4" t="n">
-        <v>23774414400</v>
-      </c>
-      <c r="DW4" t="n">
-        <v>23899066000</v>
-      </c>
-      <c r="DX4" t="n">
-        <v>23899066000</v>
-      </c>
-      <c r="DY4" t="n">
-        <v>24024761700</v>
-      </c>
-      <c r="DZ4" t="n">
-        <v>24024761700</v>
-      </c>
-      <c r="EA4" t="n">
-        <v>24150091400</v>
-      </c>
-      <c r="EB4" t="n">
-        <v>24150091400</v>
-      </c>
-      <c r="EC4" t="n">
-        <v>63280516500</v>
-      </c>
+        <v>0.190278559923172</v>
+      </c>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
+      <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="inlineStr"/>
+      <c r="CN4" t="inlineStr"/>
+      <c r="CO4" t="inlineStr"/>
+      <c r="CP4" t="inlineStr"/>
+      <c r="CQ4" t="inlineStr"/>
+      <c r="CR4" t="inlineStr"/>
+      <c r="CS4" t="inlineStr"/>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr"/>
+      <c r="CV4" t="inlineStr"/>
+      <c r="CW4" t="inlineStr"/>
+      <c r="CX4" t="inlineStr"/>
+      <c r="CY4" t="inlineStr"/>
+      <c r="CZ4" t="inlineStr"/>
+      <c r="DA4" t="inlineStr"/>
+      <c r="DB4" t="inlineStr"/>
+      <c r="DC4" t="inlineStr"/>
+      <c r="DD4" t="inlineStr"/>
+      <c r="DE4" t="inlineStr"/>
+      <c r="DF4" t="inlineStr"/>
+      <c r="DG4" t="inlineStr"/>
+      <c r="DH4" t="inlineStr"/>
+      <c r="DI4" t="inlineStr"/>
+      <c r="DJ4" t="inlineStr"/>
+      <c r="DK4" t="inlineStr"/>
+      <c r="DL4" t="inlineStr"/>
+      <c r="DM4" t="inlineStr"/>
+      <c r="DN4" t="inlineStr"/>
+      <c r="DO4" t="inlineStr"/>
+      <c r="DP4" t="inlineStr"/>
+      <c r="DQ4" t="inlineStr"/>
+      <c r="DR4" t="inlineStr"/>
+      <c r="DS4" t="inlineStr"/>
+      <c r="DT4" t="inlineStr"/>
+      <c r="DU4" t="inlineStr"/>
+      <c r="DV4" t="inlineStr"/>
+      <c r="DW4" t="inlineStr"/>
+      <c r="DX4" t="inlineStr"/>
+      <c r="DY4" t="inlineStr"/>
+      <c r="DZ4" t="inlineStr"/>
+      <c r="EA4" t="inlineStr"/>
+      <c r="EB4" t="inlineStr"/>
+      <c r="EC4" t="inlineStr"/>
+      <c r="ED4" t="inlineStr"/>
+      <c r="EE4" t="inlineStr"/>
+      <c r="EF4" t="inlineStr"/>
+      <c r="EG4" t="inlineStr"/>
+      <c r="EH4" t="inlineStr"/>
+      <c r="EI4" t="inlineStr"/>
+      <c r="EJ4" t="inlineStr"/>
+      <c r="EK4" t="inlineStr"/>
+      <c r="EL4" t="inlineStr"/>
+      <c r="EM4" t="inlineStr"/>
+      <c r="EN4" t="inlineStr"/>
+      <c r="EO4" t="inlineStr"/>
+      <c r="EP4" t="inlineStr"/>
+      <c r="EQ4" t="inlineStr"/>
+      <c r="ER4" t="inlineStr"/>
+      <c r="ES4" t="inlineStr"/>
+      <c r="ET4" t="inlineStr"/>
+      <c r="EU4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>64</v>
+        <v>0.373970091342926</v>
       </c>
       <c r="B5" t="n">
-        <v>64</v>
+        <v>0.3739697933197021</v>
       </c>
       <c r="C5" t="n">
-        <v>64</v>
+        <v>0.3739714026451111</v>
       </c>
       <c r="D5" t="n">
-        <v>64</v>
+        <v>0.3739713430404663</v>
       </c>
       <c r="E5" t="n">
-        <v>64</v>
+        <v>0.3739704191684723</v>
       </c>
       <c r="F5" t="n">
-        <v>64</v>
+        <v>0.3739715814590454</v>
       </c>
       <c r="G5" t="n">
-        <v>64</v>
+        <v>0.3739715814590454</v>
       </c>
       <c r="H5" t="n">
-        <v>64</v>
+        <v>0.3739716410636902</v>
       </c>
       <c r="I5" t="n">
-        <v>64</v>
+        <v>0.373969554901123</v>
       </c>
       <c r="J5" t="n">
-        <v>64</v>
+        <v>0.3739699423313141</v>
       </c>
       <c r="K5" t="n">
-        <v>64</v>
+        <v>0.3739703297615051</v>
       </c>
       <c r="L5" t="n">
-        <v>64</v>
+        <v>0.3739719092845917</v>
       </c>
       <c r="M5" t="n">
-        <v>64</v>
+        <v>0.3739692568778992</v>
       </c>
       <c r="N5" t="n">
-        <v>64</v>
+        <v>0.3739687204360962</v>
       </c>
       <c r="O5" t="n">
-        <v>64</v>
+        <v>0.3739712834358215</v>
       </c>
       <c r="P5" t="n">
-        <v>64</v>
+        <v>0.3739699125289917</v>
       </c>
       <c r="Q5" t="n">
-        <v>64</v>
+        <v>0.3739694952964783</v>
       </c>
       <c r="R5" t="n">
-        <v>64</v>
+        <v>0.373972475528717</v>
       </c>
       <c r="S5" t="n">
-        <v>64</v>
+        <v>0.3739722371101379</v>
       </c>
       <c r="T5" t="n">
-        <v>64</v>
+        <v>0.3739700317382812</v>
       </c>
       <c r="U5" t="n">
-        <v>64</v>
+        <v>0.3739702999591827</v>
       </c>
       <c r="V5" t="n">
-        <v>65</v>
+        <v>0.3739704489707947</v>
       </c>
       <c r="W5" t="n">
-        <v>64</v>
+        <v>0.3739703297615051</v>
       </c>
       <c r="X5" t="n">
-        <v>63</v>
+        <v>0.3739719986915588</v>
       </c>
       <c r="Y5" t="n">
-        <v>64</v>
+        <v>0.3739678859710693</v>
       </c>
       <c r="Z5" t="n">
-        <v>64</v>
+        <v>0.373970627784729</v>
       </c>
       <c r="AA5" t="n">
-        <v>64</v>
+        <v>0.3739688396453857</v>
       </c>
       <c r="AB5" t="n">
-        <v>63</v>
+        <v>0.373968243598938</v>
       </c>
       <c r="AC5" t="n">
-        <v>64</v>
+        <v>0.3739708364009857</v>
       </c>
       <c r="AD5" t="n">
-        <v>64</v>
+        <v>0.3739710748195648</v>
       </c>
       <c r="AE5" t="n">
-        <v>64</v>
+        <v>0.3739714622497559</v>
       </c>
       <c r="AF5" t="n">
-        <v>78</v>
+        <v>0.3739728629589081</v>
       </c>
       <c r="AG5" t="n">
-        <v>79</v>
+        <v>0.3739694952964783</v>
       </c>
       <c r="AH5" t="n">
-        <v>89</v>
+        <v>0.3739710450172424</v>
       </c>
       <c r="AI5" t="n">
-        <v>101</v>
+        <v>0.3743055462837219</v>
       </c>
       <c r="AJ5" t="n">
-        <v>102</v>
+        <v>0.3739693164825439</v>
       </c>
       <c r="AK5" t="n">
-        <v>112</v>
+        <v>0.3738349080085754</v>
       </c>
       <c r="AL5" t="n">
-        <v>126</v>
+        <v>0.3737640380859375</v>
       </c>
       <c r="AM5" t="n">
-        <v>137</v>
+        <v>0.3738792836666107</v>
       </c>
       <c r="AN5" t="n">
-        <v>141</v>
+        <v>0.3739708960056305</v>
       </c>
       <c r="AO5" t="n">
-        <v>145</v>
+        <v>0.3739576041698456</v>
       </c>
       <c r="AP5" t="n">
-        <v>156</v>
+        <v>0.3736016452312469</v>
       </c>
       <c r="AQ5" t="n">
-        <v>158</v>
+        <v>0.3734646439552307</v>
       </c>
       <c r="AR5" t="n">
-        <v>163</v>
+        <v>0.3731843233108521</v>
       </c>
       <c r="AS5" t="n">
-        <v>173</v>
+        <v>0.3730300664901733</v>
       </c>
       <c r="AT5" t="n">
-        <v>178</v>
+        <v>0.3730209469795227</v>
       </c>
       <c r="AU5" t="n">
-        <v>186</v>
+        <v>0.3728436827659607</v>
       </c>
       <c r="AV5" t="n">
-        <v>188</v>
+        <v>0.3728630542755127</v>
       </c>
       <c r="AW5" t="n">
-        <v>190</v>
+        <v>0.3726453185081482</v>
       </c>
       <c r="AX5" t="n">
-        <v>188</v>
+        <v>0.3724945187568665</v>
       </c>
       <c r="AY5" t="n">
-        <v>185</v>
+        <v>0.3723317980766296</v>
       </c>
       <c r="AZ5" t="n">
-        <v>182</v>
+        <v>0.371985912322998</v>
       </c>
       <c r="BA5" t="n">
-        <v>182</v>
+        <v>0.3718041777610779</v>
       </c>
       <c r="BB5" t="n">
-        <v>180</v>
+        <v>0.371557205915451</v>
       </c>
       <c r="BC5" t="n">
-        <v>178</v>
+        <v>0.3714287877082825</v>
       </c>
       <c r="BD5" t="n">
-        <v>174</v>
+        <v>0.3713581562042236</v>
       </c>
       <c r="BE5" t="n">
-        <v>170</v>
+        <v>0.3717801570892334</v>
       </c>
       <c r="BF5" t="n">
-        <v>171</v>
+        <v>0.3778453171253204</v>
       </c>
       <c r="BG5" t="n">
-        <v>170</v>
+        <v>0.3853480219841003</v>
       </c>
       <c r="BH5" t="n">
-        <v>175</v>
+        <v>0.3930789232254028</v>
       </c>
       <c r="BI5" t="n">
-        <v>171</v>
+        <v>0.3982595801353455</v>
       </c>
       <c r="BJ5" t="n">
-        <v>169</v>
+        <v>0.404346227645874</v>
       </c>
       <c r="BK5" t="n">
-        <v>171</v>
+        <v>0.4118934273719788</v>
       </c>
       <c r="BL5" t="n">
-        <v>169</v>
+        <v>0.4193663895130157</v>
       </c>
       <c r="BM5" t="n">
-        <v>169</v>
+        <v>0.4267885684967041</v>
       </c>
       <c r="BN5" t="n">
-        <v>173</v>
-      </c>
-      <c r="BO5" t="inlineStr"/>
-      <c r="BP5" t="inlineStr"/>
-      <c r="BQ5" t="inlineStr"/>
-      <c r="BR5" t="inlineStr"/>
-      <c r="BS5" t="inlineStr"/>
-      <c r="BT5" t="inlineStr"/>
-      <c r="BU5" t="inlineStr"/>
-      <c r="BV5" t="inlineStr"/>
-      <c r="BW5" t="inlineStr"/>
+        <v>0.43413907289505</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0.4416482150554657</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>0.4490522146224976</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>0.4564083516597748</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>0.4638319611549377</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>0.4714597761631012</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>0.4775876402854919</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>0.4849590659141541</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>0.4924229681491852</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>0.4986508786678314</v>
+      </c>
       <c r="BX5" t="inlineStr"/>
       <c r="BY5" t="inlineStr"/>
       <c r="BZ5" t="inlineStr"/>
@@ -2035,482 +2081,706 @@
       <c r="EA5" t="inlineStr"/>
       <c r="EB5" t="inlineStr"/>
       <c r="EC5" t="inlineStr"/>
+      <c r="ED5" t="inlineStr"/>
+      <c r="EE5" t="inlineStr"/>
+      <c r="EF5" t="inlineStr"/>
+      <c r="EG5" t="inlineStr"/>
+      <c r="EH5" t="inlineStr"/>
+      <c r="EI5" t="inlineStr"/>
+      <c r="EJ5" t="inlineStr"/>
+      <c r="EK5" t="inlineStr"/>
+      <c r="EL5" t="inlineStr"/>
+      <c r="EM5" t="inlineStr"/>
+      <c r="EN5" t="inlineStr"/>
+      <c r="EO5" t="inlineStr"/>
+      <c r="EP5" t="inlineStr"/>
+      <c r="EQ5" t="inlineStr"/>
+      <c r="ER5" t="inlineStr"/>
+      <c r="ES5" t="inlineStr"/>
+      <c r="ET5" t="inlineStr"/>
+      <c r="EU5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.06678313761949539</v>
+        <v>18780165700</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.06678939610719681</v>
+        <v>18780165700</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.06679029017686844</v>
+        <v>22052215600</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06678225100040436</v>
+        <v>22052215600</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.06678593158721924</v>
+        <v>22278400900</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.06679029017686844</v>
+        <v>22278400900</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.06679029017686844</v>
+        <v>22376785100</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.06678681820631027</v>
+        <v>22376785100</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0667850449681282</v>
+        <v>22493368000</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.0667894035577774</v>
+        <v>22493368000</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.06678682565689087</v>
+        <v>22551546900</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.06678414344787598</v>
+        <v>22551546900</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0667877197265625</v>
+        <v>22644035500</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.06678683310747147</v>
+        <v>22644035500</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.06678414344787598</v>
+        <v>22735013300</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.06678403168916702</v>
+        <v>22735013300</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.06678683310747147</v>
+        <v>22806519600</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.06678235530853271</v>
+        <v>22806519600</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.06678682565689087</v>
+        <v>22895038400</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.06678581982851028</v>
+        <v>22895038400</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.06678850203752518</v>
+        <v>22997105400</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.06678862124681473</v>
+        <v>22997105400</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.06678413599729538</v>
+        <v>23094706700</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.06678660959005356</v>
+        <v>23094706700</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.0667877197265625</v>
+        <v>23162097700</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.06678760051727295</v>
+        <v>23162097700</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.06678861379623413</v>
+        <v>23247681000</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.06678850203752518</v>
+        <v>23247681000</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.06678314507007599</v>
+        <v>23345807100</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.06681244075298309</v>
+        <v>23345807100</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.06621644645929337</v>
+        <v>23441292900</v>
       </c>
       <c r="AF6" t="n">
-        <v>-0.06313414871692657</v>
+        <v>23441292900</v>
       </c>
       <c r="AG6" t="n">
-        <v>-0.06018143147230148</v>
+        <v>23532392300</v>
       </c>
       <c r="AH6" t="n">
-        <v>-0.05690976977348328</v>
+        <v>23532392300</v>
       </c>
       <c r="AI6" t="n">
-        <v>-0.05452706664800644</v>
+        <v>23604675100</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-0.05173627287149429</v>
+        <v>23604675100</v>
       </c>
       <c r="AK6" t="n">
-        <v>-0.04931683838367462</v>
+        <v>23680124800</v>
       </c>
       <c r="AL6" t="n">
-        <v>-0.04751509428024292</v>
+        <v>23680124800</v>
       </c>
       <c r="AM6" t="n">
-        <v>-0.04600551351904869</v>
+        <v>23765098400</v>
       </c>
       <c r="AN6" t="n">
-        <v>-0.0445905327796936</v>
+        <v>23765098400</v>
       </c>
       <c r="AO6" t="n">
-        <v>-0.04438968375325203</v>
+        <v>23837413500</v>
       </c>
       <c r="AP6" t="n">
-        <v>-0.0443115271627903</v>
+        <v>23837413500</v>
       </c>
       <c r="AQ6" t="n">
-        <v>-0.04371742531657219</v>
+        <v>23917745300</v>
       </c>
       <c r="AR6" t="n">
-        <v>-0.04287426173686981</v>
+        <v>23917745300</v>
       </c>
       <c r="AS6" t="n">
-        <v>-0.04295282810926437</v>
+        <v>24020365900</v>
       </c>
       <c r="AT6" t="n">
-        <v>-0.04346687719225883</v>
+        <v>24020365900</v>
       </c>
       <c r="AU6" t="n">
-        <v>-0.04410932213068008</v>
+        <v>24118971700</v>
       </c>
       <c r="AV6" t="n">
-        <v>-0.04411892592906952</v>
+        <v>24118971700</v>
       </c>
       <c r="AW6" t="n">
-        <v>-0.04483101516962051</v>
+        <v>24217720400</v>
       </c>
       <c r="AX6" t="n">
-        <v>-0.04407943785190582</v>
+        <v>24217720400</v>
       </c>
       <c r="AY6" t="n">
-        <v>-0.04407842457294464</v>
+        <v>24323417900</v>
       </c>
       <c r="AZ6" t="n">
-        <v>-0.04393146187067032</v>
+        <v>24323417900</v>
       </c>
       <c r="BA6" t="n">
-        <v>-0.04300937429070473</v>
+        <v>24421086800</v>
       </c>
       <c r="BB6" t="n">
-        <v>-0.04288323223590851</v>
+        <v>24421086800</v>
       </c>
       <c r="BC6" t="n">
-        <v>-0.04295549541711807</v>
+        <v>24546944300</v>
       </c>
       <c r="BD6" t="n">
-        <v>-0.04316036030650139</v>
+        <v>24546944300</v>
       </c>
       <c r="BE6" t="n">
-        <v>-0.04351386055350304</v>
+        <v>24645012600</v>
       </c>
       <c r="BF6" t="n">
-        <v>-0.04327072948217392</v>
+        <v>24645012600</v>
       </c>
       <c r="BG6" t="n">
-        <v>-0.04290683940052986</v>
+        <v>24746267400</v>
       </c>
       <c r="BH6" t="n">
-        <v>-0.04248535260558128</v>
+        <v>24746267400</v>
       </c>
       <c r="BI6" t="n">
-        <v>-0.0425264947116375</v>
+        <v>24872930200</v>
       </c>
       <c r="BJ6" t="n">
-        <v>-0.04294982925057411</v>
+        <v>24872930200</v>
       </c>
       <c r="BK6" t="n">
-        <v>-0.04267653077840805</v>
+        <v>24996183900</v>
       </c>
       <c r="BL6" t="n">
-        <v>-0.04178839921951294</v>
+        <v>24996183900</v>
       </c>
       <c r="BM6" t="n">
-        <v>-0.0414135716855526</v>
+        <v>25080462200</v>
       </c>
       <c r="BN6" t="n">
-        <v>-0.04103283584117889</v>
-      </c>
-      <c r="BO6" t="inlineStr"/>
-      <c r="BP6" t="inlineStr"/>
-      <c r="BQ6" t="inlineStr"/>
-      <c r="BR6" t="inlineStr"/>
-      <c r="BS6" t="inlineStr"/>
-      <c r="BT6" t="inlineStr"/>
-      <c r="BU6" t="inlineStr"/>
-      <c r="BV6" t="inlineStr"/>
-      <c r="BW6" t="inlineStr"/>
-      <c r="BX6" t="inlineStr"/>
-      <c r="BY6" t="inlineStr"/>
-      <c r="BZ6" t="inlineStr"/>
-      <c r="CA6" t="inlineStr"/>
-      <c r="CB6" t="inlineStr"/>
-      <c r="CC6" t="inlineStr"/>
-      <c r="CD6" t="inlineStr"/>
-      <c r="CE6" t="inlineStr"/>
-      <c r="CF6" t="inlineStr"/>
-      <c r="CG6" t="inlineStr"/>
-      <c r="CH6" t="inlineStr"/>
-      <c r="CI6" t="inlineStr"/>
-      <c r="CJ6" t="inlineStr"/>
-      <c r="CK6" t="inlineStr"/>
-      <c r="CL6" t="inlineStr"/>
-      <c r="CM6" t="inlineStr"/>
-      <c r="CN6" t="inlineStr"/>
-      <c r="CO6" t="inlineStr"/>
-      <c r="CP6" t="inlineStr"/>
-      <c r="CQ6" t="inlineStr"/>
-      <c r="CR6" t="inlineStr"/>
-      <c r="CS6" t="inlineStr"/>
-      <c r="CT6" t="inlineStr"/>
-      <c r="CU6" t="inlineStr"/>
-      <c r="CV6" t="inlineStr"/>
-      <c r="CW6" t="inlineStr"/>
-      <c r="CX6" t="inlineStr"/>
-      <c r="CY6" t="inlineStr"/>
-      <c r="CZ6" t="inlineStr"/>
-      <c r="DA6" t="inlineStr"/>
-      <c r="DB6" t="inlineStr"/>
-      <c r="DC6" t="inlineStr"/>
-      <c r="DD6" t="inlineStr"/>
-      <c r="DE6" t="inlineStr"/>
-      <c r="DF6" t="inlineStr"/>
-      <c r="DG6" t="inlineStr"/>
-      <c r="DH6" t="inlineStr"/>
-      <c r="DI6" t="inlineStr"/>
-      <c r="DJ6" t="inlineStr"/>
-      <c r="DK6" t="inlineStr"/>
-      <c r="DL6" t="inlineStr"/>
-      <c r="DM6" t="inlineStr"/>
-      <c r="DN6" t="inlineStr"/>
-      <c r="DO6" t="inlineStr"/>
-      <c r="DP6" t="inlineStr"/>
-      <c r="DQ6" t="inlineStr"/>
-      <c r="DR6" t="inlineStr"/>
-      <c r="DS6" t="inlineStr"/>
-      <c r="DT6" t="inlineStr"/>
-      <c r="DU6" t="inlineStr"/>
-      <c r="DV6" t="inlineStr"/>
-      <c r="DW6" t="inlineStr"/>
-      <c r="DX6" t="inlineStr"/>
-      <c r="DY6" t="inlineStr"/>
-      <c r="DZ6" t="inlineStr"/>
-      <c r="EA6" t="inlineStr"/>
-      <c r="EB6" t="inlineStr"/>
-      <c r="EC6" t="inlineStr"/>
+        <v>25080462200</v>
+      </c>
+      <c r="BO6" t="n">
+        <v>25194818800</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>25194818800</v>
+      </c>
+      <c r="BQ6" t="n">
+        <v>25312267600</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>25312267600</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>25442147800</v>
+      </c>
+      <c r="BT6" t="n">
+        <v>25442147800</v>
+      </c>
+      <c r="BU6" t="n">
+        <v>25554796400</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>25554796400</v>
+      </c>
+      <c r="BW6" t="n">
+        <v>25668586900</v>
+      </c>
+      <c r="BX6" t="n">
+        <v>25668586900</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>25810858000</v>
+      </c>
+      <c r="BZ6" t="n">
+        <v>25810858000</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>25916133400</v>
+      </c>
+      <c r="CB6" t="n">
+        <v>25916133400</v>
+      </c>
+      <c r="CC6" t="n">
+        <v>26044915400</v>
+      </c>
+      <c r="CD6" t="n">
+        <v>26044915400</v>
+      </c>
+      <c r="CE6" t="n">
+        <v>26115482100</v>
+      </c>
+      <c r="CF6" t="n">
+        <v>26115482100</v>
+      </c>
+      <c r="CG6" t="n">
+        <v>26180892700</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>26180892700</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>26264166300</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>26264166300</v>
+      </c>
+      <c r="CK6" t="n">
+        <v>26337855900</v>
+      </c>
+      <c r="CL6" t="n">
+        <v>26337855900</v>
+      </c>
+      <c r="CM6" t="n">
+        <v>26465425200</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>26465425200</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>26588645000</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>26588645000</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>26713477600</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>26713477600</v>
+      </c>
+      <c r="CS6" t="n">
+        <v>26787731000</v>
+      </c>
+      <c r="CT6" t="n">
+        <v>26787731000</v>
+      </c>
+      <c r="CU6" t="n">
+        <v>26861142900</v>
+      </c>
+      <c r="CV6" t="n">
+        <v>26861142900</v>
+      </c>
+      <c r="CW6" t="n">
+        <v>26936224400</v>
+      </c>
+      <c r="CX6" t="n">
+        <v>26936224400</v>
+      </c>
+      <c r="CY6" t="n">
+        <v>27041674700</v>
+      </c>
+      <c r="CZ6" t="n">
+        <v>27041674700</v>
+      </c>
+      <c r="DA6" t="n">
+        <v>27166024600</v>
+      </c>
+      <c r="DB6" t="n">
+        <v>27166024600</v>
+      </c>
+      <c r="DC6" t="n">
+        <v>27234096700</v>
+      </c>
+      <c r="DD6" t="n">
+        <v>27234096700</v>
+      </c>
+      <c r="DE6" t="n">
+        <v>27309536200</v>
+      </c>
+      <c r="DF6" t="n">
+        <v>27309536200</v>
+      </c>
+      <c r="DG6" t="n">
+        <v>27381775300</v>
+      </c>
+      <c r="DH6" t="n">
+        <v>27381775300</v>
+      </c>
+      <c r="DI6" t="n">
+        <v>27462053900</v>
+      </c>
+      <c r="DJ6" t="n">
+        <v>27462053900</v>
+      </c>
+      <c r="DK6" t="n">
+        <v>27567886400</v>
+      </c>
+      <c r="DL6" t="n">
+        <v>27567886400</v>
+      </c>
+      <c r="DM6" t="n">
+        <v>27717555800</v>
+      </c>
+      <c r="DN6" t="n">
+        <v>27717555800</v>
+      </c>
+      <c r="DO6" t="n">
+        <v>27866761300</v>
+      </c>
+      <c r="DP6" t="n">
+        <v>27866761300</v>
+      </c>
+      <c r="DQ6" t="n">
+        <v>28009068100</v>
+      </c>
+      <c r="DR6" t="n">
+        <v>28009068100</v>
+      </c>
+      <c r="DS6" t="n">
+        <v>28085059600</v>
+      </c>
+      <c r="DT6" t="n">
+        <v>28085059600</v>
+      </c>
+      <c r="DU6" t="n">
+        <v>28241065800</v>
+      </c>
+      <c r="DV6" t="n">
+        <v>28241065800</v>
+      </c>
+      <c r="DW6" t="n">
+        <v>28393781000</v>
+      </c>
+      <c r="DX6" t="n">
+        <v>28393781000</v>
+      </c>
+      <c r="DY6" t="n">
+        <v>28540664100</v>
+      </c>
+      <c r="DZ6" t="n">
+        <v>28540664100</v>
+      </c>
+      <c r="EA6" t="n">
+        <v>28692842200</v>
+      </c>
+      <c r="EB6" t="n">
+        <v>28692842200</v>
+      </c>
+      <c r="EC6" t="n">
+        <v>28842540700</v>
+      </c>
+      <c r="ED6" t="n">
+        <v>28842540700</v>
+      </c>
+      <c r="EE6" t="n">
+        <v>28985980100</v>
+      </c>
+      <c r="EF6" t="n">
+        <v>28985980100</v>
+      </c>
+      <c r="EG6" t="n">
+        <v>29145233200</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>29145233200</v>
+      </c>
+      <c r="EI6" t="n">
+        <v>29291400700</v>
+      </c>
+      <c r="EJ6" t="n">
+        <v>29291400700</v>
+      </c>
+      <c r="EK6" t="n">
+        <v>29445217400</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>29445217400</v>
+      </c>
+      <c r="EM6" t="n">
+        <v>29592607900</v>
+      </c>
+      <c r="EN6" t="n">
+        <v>29592607900</v>
+      </c>
+      <c r="EO6" t="n">
+        <v>29715489500</v>
+      </c>
+      <c r="EP6" t="n">
+        <v>29715489500</v>
+      </c>
+      <c r="EQ6" t="n">
+        <v>29866018900</v>
+      </c>
+      <c r="ER6" t="n">
+        <v>29866018900</v>
+      </c>
+      <c r="ES6" t="n">
+        <v>30015984900</v>
+      </c>
+      <c r="ET6" t="n">
+        <v>30015984900</v>
+      </c>
+      <c r="EU6" t="n">
+        <v>68799082000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>-123</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-125</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-125</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-123</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-123</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="S7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="U7" t="n">
+        <v>-123</v>
+      </c>
+      <c r="V7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="X7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>-123</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>-124</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>-123</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>-125</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>-121</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>-110</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>-108</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>-91</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>-88</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>-77</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>-73</v>
+      </c>
+      <c r="AQ7" t="n">
         <v>-65</v>
       </c>
-      <c r="B7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-64</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="K7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="L7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="N7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="P7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="R7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="S7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="T7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="U7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="V7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="W7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="X7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>-65</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>-67</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>-58</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>-48</v>
-      </c>
-      <c r="AI7" t="n">
+      <c r="AR7" t="n">
+        <v>-59</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>-55</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>-42</v>
+      </c>
+      <c r="AU7" t="n">
         <v>-37</v>
       </c>
-      <c r="AJ7" t="n">
-        <v>-28</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>-22</v>
-      </c>
-      <c r="AL7" t="n">
+      <c r="AV7" t="n">
+        <v>-26</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>-21</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>-13</v>
+      </c>
+      <c r="AY7" t="n">
         <v>-11</v>
       </c>
-      <c r="AM7" t="n">
+      <c r="AZ7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>4</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>6</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>8</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>10</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>10</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>-2</v>
+      </c>
+      <c r="BM7" t="n">
         <v>-4</v>
       </c>
-      <c r="AN7" t="n">
+      <c r="BN7" t="n">
+        <v>-4</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP7" t="n">
         <v>3</v>
       </c>
-      <c r="AO7" t="n">
-        <v>5</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>6</v>
-      </c>
-      <c r="AQ7" t="n">
+      <c r="BQ7" t="n">
         <v>7</v>
       </c>
-      <c r="AR7" t="n">
-        <v>7</v>
-      </c>
-      <c r="AS7" t="n">
-        <v>13</v>
-      </c>
-      <c r="AT7" t="n">
-        <v>12</v>
-      </c>
-      <c r="AU7" t="n">
+      <c r="BR7" t="n">
+        <v>4</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BT7" t="n">
         <v>8</v>
       </c>
-      <c r="AV7" t="n">
-        <v>6</v>
-      </c>
-      <c r="AW7" t="n">
-        <v>3</v>
-      </c>
-      <c r="AX7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY7" t="n">
+      <c r="BU7" t="n">
         <v>0</v>
       </c>
-      <c r="AZ7" t="n">
-        <v>6</v>
-      </c>
-      <c r="BA7" t="n">
+      <c r="BV7" t="n">
         <v>2</v>
       </c>
-      <c r="BB7" t="n">
-        <v>6</v>
-      </c>
-      <c r="BC7" t="n">
-        <v>11</v>
-      </c>
-      <c r="BD7" t="n">
-        <v>10</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>2</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>4</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>5</v>
-      </c>
-      <c r="BI7" t="n">
-        <v>3</v>
-      </c>
-      <c r="BJ7" t="n">
-        <v>4</v>
-      </c>
-      <c r="BK7" t="n">
+      <c r="BW7" t="n">
         <v>0</v>
       </c>
-      <c r="BL7" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM7" t="n">
-        <v>2</v>
-      </c>
-      <c r="BN7" t="n">
-        <v>8</v>
-      </c>
-      <c r="BO7" t="inlineStr"/>
-      <c r="BP7" t="inlineStr"/>
-      <c r="BQ7" t="inlineStr"/>
-      <c r="BR7" t="inlineStr"/>
-      <c r="BS7" t="inlineStr"/>
-      <c r="BT7" t="inlineStr"/>
-      <c r="BU7" t="inlineStr"/>
-      <c r="BV7" t="inlineStr"/>
-      <c r="BW7" t="inlineStr"/>
       <c r="BX7" t="inlineStr"/>
       <c r="BY7" t="inlineStr"/>
       <c r="BZ7" t="inlineStr"/>
@@ -2569,6 +2839,24 @@
       <c r="EA7" t="inlineStr"/>
       <c r="EB7" t="inlineStr"/>
       <c r="EC7" t="inlineStr"/>
+      <c r="ED7" t="inlineStr"/>
+      <c r="EE7" t="inlineStr"/>
+      <c r="EF7" t="inlineStr"/>
+      <c r="EG7" t="inlineStr"/>
+      <c r="EH7" t="inlineStr"/>
+      <c r="EI7" t="inlineStr"/>
+      <c r="EJ7" t="inlineStr"/>
+      <c r="EK7" t="inlineStr"/>
+      <c r="EL7" t="inlineStr"/>
+      <c r="EM7" t="inlineStr"/>
+      <c r="EN7" t="inlineStr"/>
+      <c r="EO7" t="inlineStr"/>
+      <c r="EP7" t="inlineStr"/>
+      <c r="EQ7" t="inlineStr"/>
+      <c r="ER7" t="inlineStr"/>
+      <c r="ES7" t="inlineStr"/>
+      <c r="ET7" t="inlineStr"/>
+      <c r="EU7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: Continuous detection and removal
</commit_message>
<xml_diff>
--- a/weedDepthTake3.xlsx
+++ b/weedDepthTake3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EU7"/>
+  <dimension ref="A1:FW7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,247 +887,359 @@
       <c r="EU1" s="1" t="n">
         <v>150</v>
       </c>
+      <c r="EV1" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="EW1" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="EX1" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="EY1" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="EZ1" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="FA1" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="FB1" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="FC1" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="FD1" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="FE1" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="FF1" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="FG1" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="FH1" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="FI1" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="FJ1" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="FK1" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="FL1" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="FM1" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="FN1" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="FO1" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="FP1" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="FQ1" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="FR1" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="FS1" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="FT1" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="FU1" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="FV1" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="FW1" s="1" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.0672764927148819</v>
+        <v>0.2518116533756256</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.06727827340364456</v>
+        <v>0.2518061995506287</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.06727313995361328</v>
+        <v>0.2518115639686584</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.06727314740419388</v>
+        <v>0.2518103420734406</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.06727760285139084</v>
+        <v>0.2518114447593689</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.06727225333452225</v>
+        <v>0.2518038749694824</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.06727474927902222</v>
+        <v>0.2518133223056793</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.06727492064237595</v>
+        <v>0.2518078684806824</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0672793835401535</v>
+        <v>0.2518119513988495</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.06727046519517899</v>
+        <v>0.2518056333065033</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.06726868450641632</v>
+        <v>0.2518079280853271</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.06727582216262817</v>
+        <v>0.2518086135387421</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.06728094816207886</v>
+        <v>0.2518084347248077</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.0672764927148819</v>
+        <v>0.2518051564693451</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.06727582216262817</v>
+        <v>0.2518114149570465</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.06727413833141327</v>
+        <v>0.2518081367015839</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.06727314740419388</v>
+        <v>0.2518080770969391</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.06727313995361328</v>
+        <v>0.2518091201782227</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.06727760285139084</v>
+        <v>0.2518055438995361</v>
       </c>
       <c r="T2" t="n">
-        <v>-0.06728184223175049</v>
+        <v>0.2518084049224854</v>
       </c>
       <c r="U2" t="n">
-        <v>-0.06727564334869385</v>
+        <v>0.2518075406551361</v>
       </c>
       <c r="V2" t="n">
-        <v>-0.06727760285139084</v>
+        <v>0.25180983543396</v>
       </c>
       <c r="W2" t="n">
-        <v>-0.06727848947048187</v>
+        <v>0.251810759305954</v>
       </c>
       <c r="X2" t="n">
-        <v>-0.06727307289838791</v>
+        <v>0.2518064677715302</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0.06727580726146698</v>
+        <v>0.2518094778060913</v>
       </c>
       <c r="Z2" t="n">
-        <v>-0.0672764927148819</v>
+        <v>0.251807689666748</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.06727670878171921</v>
+        <v>0.25180384516716</v>
       </c>
       <c r="AB2" t="n">
-        <v>-0.06727916747331619</v>
+        <v>0.251808226108551</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.06727564334869385</v>
+        <v>0.2518104910850525</v>
       </c>
       <c r="AD2" t="n">
-        <v>-0.06727759540081024</v>
+        <v>0.2518101334571838</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.06727207452058792</v>
+        <v>0.2518084943294525</v>
       </c>
       <c r="AF2" t="n">
-        <v>-0.06727474927902222</v>
+        <v>0.2518093585968018</v>
       </c>
       <c r="AG2" t="n">
-        <v>-0.06727564334869385</v>
+        <v>0.2518050968647003</v>
       </c>
       <c r="AH2" t="n">
-        <v>-0.06726551055908203</v>
+        <v>0.2518068253993988</v>
       </c>
       <c r="AI2" t="n">
-        <v>-0.06518979370594025</v>
+        <v>0.2518092095851898</v>
       </c>
       <c r="AJ2" t="n">
-        <v>-0.0625062957406044</v>
+        <v>0.2517746388912201</v>
       </c>
       <c r="AK2" t="n">
-        <v>-0.06142423674464226</v>
+        <v>0.2492293417453766</v>
       </c>
       <c r="AL2" t="n">
-        <v>-0.05851275473833084</v>
+        <v>0.2458909451961517</v>
       </c>
       <c r="AM2" t="n">
-        <v>-0.0563330166041851</v>
+        <v>0.2431709170341492</v>
       </c>
       <c r="AN2" t="n">
-        <v>-0.05344094336032867</v>
+        <v>0.2390767782926559</v>
       </c>
       <c r="AO2" t="n">
-        <v>-0.05145208165049553</v>
+        <v>0.2364064455032349</v>
       </c>
       <c r="AP2" t="n">
-        <v>-0.04987892135977745</v>
+        <v>0.2343425452709198</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.04868118092417717</v>
+        <v>0.2322858721017838</v>
       </c>
       <c r="AR2" t="n">
-        <v>-0.04694539308547974</v>
+        <v>0.2298557758331299</v>
       </c>
       <c r="AS2" t="n">
-        <v>-0.04474370554089546</v>
+        <v>0.2274951487779617</v>
       </c>
       <c r="AT2" t="n">
-        <v>-0.04258942231535912</v>
+        <v>0.224357008934021</v>
       </c>
       <c r="AU2" t="n">
-        <v>-0.04029867425560951</v>
+        <v>0.2217260748147964</v>
       </c>
       <c r="AV2" t="n">
-        <v>-0.03770944476127625</v>
+        <v>0.2195723652839661</v>
       </c>
       <c r="AW2" t="n">
-        <v>-0.03614207729697227</v>
+        <v>0.2168182879686356</v>
       </c>
       <c r="AX2" t="n">
-        <v>-0.03492633625864983</v>
+        <v>0.2145716995000839</v>
       </c>
       <c r="AY2" t="n">
-        <v>-0.03428634256124496</v>
+        <v>0.2131835669279099</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-0.03292278200387955</v>
+        <v>0.2112781852483749</v>
       </c>
       <c r="BA2" t="n">
-        <v>-0.03226296603679657</v>
+        <v>0.2101307064294815</v>
       </c>
       <c r="BB2" t="n">
-        <v>-0.03195701912045479</v>
+        <v>0.2093961834907532</v>
       </c>
       <c r="BC2" t="n">
-        <v>-0.03162122517824173</v>
+        <v>0.2086460739374161</v>
       </c>
       <c r="BD2" t="n">
-        <v>-0.0312182791531086</v>
+        <v>0.2085623443126678</v>
       </c>
       <c r="BE2" t="n">
-        <v>-0.03113839030265808</v>
+        <v>0.2087182253599167</v>
       </c>
       <c r="BF2" t="n">
-        <v>-0.0301157683134079</v>
+        <v>0.2095913738012314</v>
       </c>
       <c r="BG2" t="n">
-        <v>-0.02959166839718819</v>
+        <v>0.209787905216217</v>
       </c>
       <c r="BH2" t="n">
-        <v>-0.029451048001647</v>
+        <v>0.2098500579595566</v>
       </c>
       <c r="BI2" t="n">
-        <v>-0.02966141887009144</v>
+        <v>0.2101480215787888</v>
       </c>
       <c r="BJ2" t="n">
-        <v>-0.02998756244778633</v>
+        <v>0.2101963013410568</v>
       </c>
       <c r="BK2" t="n">
-        <v>-0.03002091869711876</v>
+        <v>0.2096040844917297</v>
       </c>
       <c r="BL2" t="n">
-        <v>-0.03003714606165886</v>
+        <v>0.2092240303754807</v>
       </c>
       <c r="BM2" t="n">
-        <v>-0.03010239824652672</v>
+        <v>0.2092225104570389</v>
       </c>
       <c r="BN2" t="n">
-        <v>-0.02857845276594162</v>
+        <v>0.2090925425291061</v>
       </c>
       <c r="BO2" t="n">
-        <v>-0.02759779989719391</v>
+        <v>0.2085836082696915</v>
       </c>
       <c r="BP2" t="n">
-        <v>-0.02669366076588631</v>
+        <v>0.2084452360868454</v>
       </c>
       <c r="BQ2" t="n">
-        <v>-0.02627201750874519</v>
+        <v>0.2517973482608795</v>
       </c>
       <c r="BR2" t="n">
-        <v>-0.02549014985561371</v>
+        <v>0.2485003769397736</v>
       </c>
       <c r="BS2" t="n">
-        <v>-0.0251185167580843</v>
+        <v>0.2437108308076859</v>
       </c>
       <c r="BT2" t="n">
-        <v>-0.0251725111156702</v>
+        <v>0.2400694340467453</v>
       </c>
       <c r="BU2" t="n">
-        <v>-0.02493898198008537</v>
+        <v>0.2363931238651276</v>
       </c>
       <c r="BV2" t="n">
-        <v>-0.02449499070644379</v>
+        <v>0.2331372797489166</v>
       </c>
       <c r="BW2" t="n">
-        <v>-0.0234505906701088</v>
-      </c>
-      <c r="BX2" t="inlineStr"/>
-      <c r="BY2" t="inlineStr"/>
-      <c r="BZ2" t="inlineStr"/>
-      <c r="CA2" t="inlineStr"/>
-      <c r="CB2" t="inlineStr"/>
-      <c r="CC2" t="inlineStr"/>
-      <c r="CD2" t="inlineStr"/>
-      <c r="CE2" t="inlineStr"/>
-      <c r="CF2" t="inlineStr"/>
-      <c r="CG2" t="inlineStr"/>
-      <c r="CH2" t="inlineStr"/>
-      <c r="CI2" t="inlineStr"/>
-      <c r="CJ2" t="inlineStr"/>
-      <c r="CK2" t="inlineStr"/>
+        <v>0.2298998236656189</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>0.2266610264778137</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>0.2234226763248444</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>0.2198142260313034</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0.2168450951576233</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.2149937301874161</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>0.2132111191749573</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>0.2121186405420303</v>
+      </c>
+      <c r="CE2" t="n">
+        <v>0.210922047495842</v>
+      </c>
+      <c r="CF2" t="n">
+        <v>0.2100589573383331</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>0.210081472992897</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>0.2098067551851273</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>0.2094677984714508</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>0.2092708796262741</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.2094676792621613</v>
+      </c>
       <c r="CL2" t="inlineStr"/>
       <c r="CM2" t="inlineStr"/>
       <c r="CN2" t="inlineStr"/>
@@ -1190,247 +1302,303 @@
       <c r="ES2" t="inlineStr"/>
       <c r="ET2" t="inlineStr"/>
       <c r="EU2" t="inlineStr"/>
+      <c r="EV2" t="inlineStr"/>
+      <c r="EW2" t="inlineStr"/>
+      <c r="EX2" t="inlineStr"/>
+      <c r="EY2" t="inlineStr"/>
+      <c r="EZ2" t="inlineStr"/>
+      <c r="FA2" t="inlineStr"/>
+      <c r="FB2" t="inlineStr"/>
+      <c r="FC2" t="inlineStr"/>
+      <c r="FD2" t="inlineStr"/>
+      <c r="FE2" t="inlineStr"/>
+      <c r="FF2" t="inlineStr"/>
+      <c r="FG2" t="inlineStr"/>
+      <c r="FH2" t="inlineStr"/>
+      <c r="FI2" t="inlineStr"/>
+      <c r="FJ2" t="inlineStr"/>
+      <c r="FK2" t="inlineStr"/>
+      <c r="FL2" t="inlineStr"/>
+      <c r="FM2" t="inlineStr"/>
+      <c r="FN2" t="inlineStr"/>
+      <c r="FO2" t="inlineStr"/>
+      <c r="FP2" t="inlineStr"/>
+      <c r="FQ2" t="inlineStr"/>
+      <c r="FR2" t="inlineStr"/>
+      <c r="FS2" t="inlineStr"/>
+      <c r="FT2" t="inlineStr"/>
+      <c r="FU2" t="inlineStr"/>
+      <c r="FV2" t="inlineStr"/>
+      <c r="FW2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>258</v>
+        <v>0.3738269507884979</v>
       </c>
       <c r="B3" t="n">
-        <v>258</v>
+        <v>0.3738243579864502</v>
       </c>
       <c r="C3" t="n">
-        <v>258</v>
+        <v>0.3738259077072144</v>
       </c>
       <c r="D3" t="n">
-        <v>258</v>
+        <v>0.3738263249397278</v>
       </c>
       <c r="E3" t="n">
-        <v>258</v>
+        <v>0.3738232851028442</v>
       </c>
       <c r="F3" t="n">
-        <v>258</v>
+        <v>0.3738230466842651</v>
       </c>
       <c r="G3" t="n">
-        <v>258</v>
+        <v>0.3738260865211487</v>
       </c>
       <c r="H3" t="n">
-        <v>258</v>
+        <v>0.3738259375095367</v>
       </c>
       <c r="I3" t="n">
-        <v>258</v>
+        <v>0.3738252520561218</v>
       </c>
       <c r="J3" t="n">
-        <v>258</v>
+        <v>0.3738245368003845</v>
       </c>
       <c r="K3" t="n">
-        <v>258</v>
+        <v>0.3738239407539368</v>
       </c>
       <c r="L3" t="n">
-        <v>258</v>
+        <v>0.3738243579864502</v>
       </c>
       <c r="M3" t="n">
-        <v>258</v>
+        <v>0.3738252520561218</v>
       </c>
       <c r="N3" t="n">
-        <v>258</v>
+        <v>0.3738247156143188</v>
       </c>
       <c r="O3" t="n">
-        <v>258</v>
+        <v>0.3738273084163666</v>
       </c>
       <c r="P3" t="n">
-        <v>258</v>
+        <v>0.373823881149292</v>
       </c>
       <c r="Q3" t="n">
-        <v>259</v>
+        <v>0.3738235533237457</v>
       </c>
       <c r="R3" t="n">
-        <v>258</v>
+        <v>0.3738251328468323</v>
       </c>
       <c r="S3" t="n">
-        <v>259</v>
+        <v>0.3738245368003845</v>
       </c>
       <c r="T3" t="n">
-        <v>259</v>
+        <v>0.3738242983818054</v>
       </c>
       <c r="U3" t="n">
-        <v>258</v>
+        <v>0.373824417591095</v>
       </c>
       <c r="V3" t="n">
-        <v>258</v>
+        <v>0.3738263547420502</v>
       </c>
       <c r="W3" t="n">
-        <v>258</v>
+        <v>0.3738253116607666</v>
       </c>
       <c r="X3" t="n">
-        <v>258</v>
+        <v>0.3738266229629517</v>
       </c>
       <c r="Y3" t="n">
-        <v>258</v>
+        <v>0.3738241493701935</v>
       </c>
       <c r="Z3" t="n">
-        <v>258</v>
+        <v>0.3738248646259308</v>
       </c>
       <c r="AA3" t="n">
-        <v>258</v>
+        <v>0.373822420835495</v>
       </c>
       <c r="AB3" t="n">
-        <v>258</v>
+        <v>0.3738249242305756</v>
       </c>
       <c r="AC3" t="n">
-        <v>259</v>
+        <v>0.3738249242305756</v>
       </c>
       <c r="AD3" t="n">
-        <v>258</v>
+        <v>0.373824417591095</v>
       </c>
       <c r="AE3" t="n">
-        <v>258</v>
+        <v>0.3738256096839905</v>
       </c>
       <c r="AF3" t="n">
-        <v>258</v>
+        <v>0.373824268579483</v>
       </c>
       <c r="AG3" t="n">
-        <v>259</v>
+        <v>0.3738240599632263</v>
       </c>
       <c r="AH3" t="n">
-        <v>258</v>
+        <v>0.3738250136375427</v>
       </c>
       <c r="AI3" t="n">
-        <v>259</v>
+        <v>0.3738214671611786</v>
       </c>
       <c r="AJ3" t="n">
-        <v>257</v>
+        <v>0.3738290071487427</v>
       </c>
       <c r="AK3" t="n">
-        <v>248</v>
+        <v>0.3736947774887085</v>
       </c>
       <c r="AL3" t="n">
-        <v>244</v>
+        <v>0.3740843534469604</v>
       </c>
       <c r="AM3" t="n">
-        <v>241</v>
+        <v>0.3740297555923462</v>
       </c>
       <c r="AN3" t="n">
-        <v>238</v>
+        <v>0.3737812042236328</v>
       </c>
       <c r="AO3" t="n">
-        <v>233</v>
+        <v>0.3734385371208191</v>
       </c>
       <c r="AP3" t="n">
-        <v>230</v>
+        <v>0.3731780648231506</v>
       </c>
       <c r="AQ3" t="n">
-        <v>228</v>
+        <v>0.3733046650886536</v>
       </c>
       <c r="AR3" t="n">
-        <v>225</v>
+        <v>0.3732152283191681</v>
       </c>
       <c r="AS3" t="n">
-        <v>228</v>
+        <v>0.3730510175228119</v>
       </c>
       <c r="AT3" t="n">
-        <v>220</v>
+        <v>0.3728269934654236</v>
       </c>
       <c r="AU3" t="n">
-        <v>216</v>
+        <v>0.3725806474685669</v>
       </c>
       <c r="AV3" t="n">
-        <v>209</v>
+        <v>0.3724945783615112</v>
       </c>
       <c r="AW3" t="n">
-        <v>210</v>
+        <v>0.3722658157348633</v>
       </c>
       <c r="AX3" t="n">
-        <v>204</v>
+        <v>0.3721331655979156</v>
       </c>
       <c r="AY3" t="n">
-        <v>201</v>
+        <v>0.3758062720298767</v>
       </c>
       <c r="AZ3" t="n">
-        <v>199</v>
+        <v>0.3813859224319458</v>
       </c>
       <c r="BA3" t="n">
-        <v>197</v>
+        <v>0.3877924680709839</v>
       </c>
       <c r="BB3" t="n">
-        <v>197</v>
+        <v>0.3941441178321838</v>
       </c>
       <c r="BC3" t="n">
-        <v>192</v>
+        <v>0.4017126858234406</v>
       </c>
       <c r="BD3" t="n">
-        <v>190</v>
+        <v>0.408197283744812</v>
       </c>
       <c r="BE3" t="n">
-        <v>191</v>
+        <v>0.4168115258216858</v>
       </c>
       <c r="BF3" t="n">
-        <v>182</v>
+        <v>0.4258450269699097</v>
       </c>
       <c r="BG3" t="n">
-        <v>174</v>
+        <v>0.4330894351005554</v>
       </c>
       <c r="BH3" t="n">
-        <v>172</v>
+        <v>0.4396384954452515</v>
       </c>
       <c r="BI3" t="n">
-        <v>172</v>
+        <v>0.4458955824375153</v>
       </c>
       <c r="BJ3" t="n">
-        <v>172</v>
+        <v>0.4520291090011597</v>
       </c>
       <c r="BK3" t="n">
-        <v>171</v>
+        <v>0.458171010017395</v>
       </c>
       <c r="BL3" t="n">
-        <v>172</v>
+        <v>0.4658509492874146</v>
       </c>
       <c r="BM3" t="n">
-        <v>170</v>
+        <v>0.4745189547538757</v>
       </c>
       <c r="BN3" t="n">
-        <v>168</v>
+        <v>0.4832828938961029</v>
       </c>
       <c r="BO3" t="n">
-        <v>169</v>
+        <v>0.4908609390258789</v>
       </c>
       <c r="BP3" t="n">
-        <v>166</v>
+        <v>0.4984065294265747</v>
       </c>
       <c r="BQ3" t="n">
-        <v>166</v>
+        <v>0.3738182783126831</v>
       </c>
       <c r="BR3" t="n">
-        <v>165</v>
+        <v>0.3737271428108215</v>
       </c>
       <c r="BS3" t="n">
-        <v>166</v>
+        <v>0.3739233613014221</v>
       </c>
       <c r="BT3" t="n">
-        <v>167</v>
+        <v>0.3737149834632874</v>
       </c>
       <c r="BU3" t="n">
-        <v>166</v>
+        <v>0.3734302520751953</v>
       </c>
       <c r="BV3" t="n">
-        <v>165</v>
+        <v>0.3733440041542053</v>
       </c>
       <c r="BW3" t="n">
-        <v>163</v>
-      </c>
-      <c r="BX3" t="inlineStr"/>
-      <c r="BY3" t="inlineStr"/>
-      <c r="BZ3" t="inlineStr"/>
-      <c r="CA3" t="inlineStr"/>
-      <c r="CB3" t="inlineStr"/>
-      <c r="CC3" t="inlineStr"/>
-      <c r="CD3" t="inlineStr"/>
-      <c r="CE3" t="inlineStr"/>
-      <c r="CF3" t="inlineStr"/>
-      <c r="CG3" t="inlineStr"/>
-      <c r="CH3" t="inlineStr"/>
-      <c r="CI3" t="inlineStr"/>
-      <c r="CJ3" t="inlineStr"/>
-      <c r="CK3" t="inlineStr"/>
+        <v>0.373136579990387</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>0.3729794025421143</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>0.372547447681427</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>0.3724917769432068</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>0.3722875118255615</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>0.3726269006729126</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>0.3769407272338867</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>0.3828717470169067</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>0.3891350626945496</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>0.3952606320381165</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>0.4017727971076965</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>0.4093599319458008</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>0.4156818389892578</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>0.4218723773956299</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>0.4283828437328339</v>
+      </c>
       <c r="CL3" t="inlineStr"/>
       <c r="CM3" t="inlineStr"/>
       <c r="CN3" t="inlineStr"/>
@@ -1493,247 +1661,303 @@
       <c r="ES3" t="inlineStr"/>
       <c r="ET3" t="inlineStr"/>
       <c r="EU3" t="inlineStr"/>
+      <c r="EV3" t="inlineStr"/>
+      <c r="EW3" t="inlineStr"/>
+      <c r="EX3" t="inlineStr"/>
+      <c r="EY3" t="inlineStr"/>
+      <c r="EZ3" t="inlineStr"/>
+      <c r="FA3" t="inlineStr"/>
+      <c r="FB3" t="inlineStr"/>
+      <c r="FC3" t="inlineStr"/>
+      <c r="FD3" t="inlineStr"/>
+      <c r="FE3" t="inlineStr"/>
+      <c r="FF3" t="inlineStr"/>
+      <c r="FG3" t="inlineStr"/>
+      <c r="FH3" t="inlineStr"/>
+      <c r="FI3" t="inlineStr"/>
+      <c r="FJ3" t="inlineStr"/>
+      <c r="FK3" t="inlineStr"/>
+      <c r="FL3" t="inlineStr"/>
+      <c r="FM3" t="inlineStr"/>
+      <c r="FN3" t="inlineStr"/>
+      <c r="FO3" t="inlineStr"/>
+      <c r="FP3" t="inlineStr"/>
+      <c r="FQ3" t="inlineStr"/>
+      <c r="FR3" t="inlineStr"/>
+      <c r="FS3" t="inlineStr"/>
+      <c r="FT3" t="inlineStr"/>
+      <c r="FU3" t="inlineStr"/>
+      <c r="FV3" t="inlineStr"/>
+      <c r="FW3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.2518490850925446</v>
+        <v>134</v>
       </c>
       <c r="B4" t="n">
-        <v>0.2518492043018341</v>
+        <v>134</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2518498003482819</v>
+        <v>134</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2518519163131714</v>
+        <v>134</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2518483698368073</v>
+        <v>134</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2518510520458221</v>
+        <v>134</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2518507242202759</v>
+        <v>135</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2518466711044312</v>
+        <v>134</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2518490254878998</v>
+        <v>134</v>
       </c>
       <c r="J4" t="n">
-        <v>0.251846581697464</v>
+        <v>134</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2518476247787476</v>
+        <v>134</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2518509924411774</v>
+        <v>134</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2518505752086639</v>
+        <v>134</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2518472671508789</v>
+        <v>134</v>
       </c>
       <c r="O4" t="n">
-        <v>0.251848578453064</v>
+        <v>134</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2518452703952789</v>
+        <v>134</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2518473565578461</v>
+        <v>134</v>
       </c>
       <c r="R4" t="n">
-        <v>0.2518517374992371</v>
+        <v>134</v>
       </c>
       <c r="S4" t="n">
-        <v>0.2518488466739655</v>
+        <v>134</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2518502771854401</v>
+        <v>135</v>
       </c>
       <c r="U4" t="n">
-        <v>0.2518540322780609</v>
+        <v>134</v>
       </c>
       <c r="V4" t="n">
-        <v>0.2518505156040192</v>
+        <v>134</v>
       </c>
       <c r="W4" t="n">
-        <v>0.2518478333950043</v>
+        <v>134</v>
       </c>
       <c r="X4" t="n">
-        <v>0.2518524825572968</v>
+        <v>134</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.2518487572669983</v>
+        <v>134</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.251849353313446</v>
+        <v>134</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2518483400344849</v>
+        <v>134</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.2518493831157684</v>
+        <v>135</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.2518513798713684</v>
+        <v>134</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.2518508434295654</v>
+        <v>134</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.2518494427204132</v>
+        <v>134</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.2518534362316132</v>
+        <v>134</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.2518503367900848</v>
+        <v>134</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.2518687546253204</v>
+        <v>134</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.2506610453128815</v>
+        <v>134</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.2473911494016647</v>
+        <v>134</v>
       </c>
       <c r="AK4" t="n">
-        <v>0.2456622719764709</v>
+        <v>134</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.2428667396306992</v>
+        <v>123</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.240818589925766</v>
+        <v>120</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.2385523617267609</v>
+        <v>118</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.2366505563259125</v>
+        <v>109</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.2350364923477173</v>
+        <v>105</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.2332315891981125</v>
+        <v>100</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.2316875606775284</v>
+        <v>89</v>
       </c>
       <c r="AS4" t="n">
-        <v>0.2294118404388428</v>
+        <v>81</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.2275154888629913</v>
+        <v>74</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.2250328361988068</v>
+        <v>71</v>
       </c>
       <c r="AV4" t="n">
-        <v>0.2231327444314957</v>
+        <v>56</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.2217909246683121</v>
+        <v>52</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.2200163602828979</v>
+        <v>45</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.2184580415487289</v>
+        <v>34</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.2161207944154739</v>
+        <v>33</v>
       </c>
       <c r="BA4" t="n">
-        <v>0.2143111526966095</v>
+        <v>28</v>
       </c>
       <c r="BB4" t="n">
-        <v>0.2132555842399597</v>
+        <v>18</v>
       </c>
       <c r="BC4" t="n">
-        <v>0.2115977257490158</v>
+        <v>18</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.2106547504663467</v>
+        <v>13</v>
       </c>
       <c r="BE4" t="n">
-        <v>0.2092414796352386</v>
+        <v>13</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.2067586034536362</v>
+        <v>20</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.2042021900415421</v>
+        <v>19</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.2029288858175278</v>
+        <v>18</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.2020822763442993</v>
+        <v>22</v>
       </c>
       <c r="BJ4" t="n">
-        <v>0.2012858092784882</v>
+        <v>24</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.1997993439435959</v>
+        <v>24</v>
       </c>
       <c r="BL4" t="n">
-        <v>0.1989577561616898</v>
+        <v>23</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.1981549561023712</v>
+        <v>24</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.1966294199228287</v>
+        <v>24</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.196053609251976</v>
+        <v>22</v>
       </c>
       <c r="BP4" t="n">
-        <v>0.1952443271875381</v>
+        <v>18</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0.1943223029375076</v>
+        <v>128</v>
       </c>
       <c r="BR4" t="n">
-        <v>0.1934070438146591</v>
+        <v>129</v>
       </c>
       <c r="BS4" t="n">
-        <v>0.1927557736635208</v>
+        <v>123</v>
       </c>
       <c r="BT4" t="n">
-        <v>0.1922584176063538</v>
+        <v>116</v>
       </c>
       <c r="BU4" t="n">
-        <v>0.1916122436523438</v>
+        <v>107</v>
       </c>
       <c r="BV4" t="n">
-        <v>0.1909289360046387</v>
+        <v>101</v>
       </c>
       <c r="BW4" t="n">
-        <v>0.190278559923172</v>
-      </c>
-      <c r="BX4" t="inlineStr"/>
-      <c r="BY4" t="inlineStr"/>
-      <c r="BZ4" t="inlineStr"/>
-      <c r="CA4" t="inlineStr"/>
-      <c r="CB4" t="inlineStr"/>
-      <c r="CC4" t="inlineStr"/>
-      <c r="CD4" t="inlineStr"/>
-      <c r="CE4" t="inlineStr"/>
-      <c r="CF4" t="inlineStr"/>
-      <c r="CG4" t="inlineStr"/>
-      <c r="CH4" t="inlineStr"/>
-      <c r="CI4" t="inlineStr"/>
-      <c r="CJ4" t="inlineStr"/>
-      <c r="CK4" t="inlineStr"/>
+        <v>97</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>82</v>
+      </c>
+      <c r="BY4" t="n">
+        <v>74</v>
+      </c>
+      <c r="BZ4" t="n">
+        <v>57</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>49</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>39</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>33</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>31</v>
+      </c>
+      <c r="CE4" t="n">
+        <v>26</v>
+      </c>
+      <c r="CF4" t="n">
+        <v>21</v>
+      </c>
+      <c r="CG4" t="n">
+        <v>22</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>19</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>16</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>16</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>14</v>
+      </c>
       <c r="CL4" t="inlineStr"/>
       <c r="CM4" t="inlineStr"/>
       <c r="CN4" t="inlineStr"/>
@@ -1796,1005 +2020,1201 @@
       <c r="ES4" t="inlineStr"/>
       <c r="ET4" t="inlineStr"/>
       <c r="EU4" t="inlineStr"/>
+      <c r="EV4" t="inlineStr"/>
+      <c r="EW4" t="inlineStr"/>
+      <c r="EX4" t="inlineStr"/>
+      <c r="EY4" t="inlineStr"/>
+      <c r="EZ4" t="inlineStr"/>
+      <c r="FA4" t="inlineStr"/>
+      <c r="FB4" t="inlineStr"/>
+      <c r="FC4" t="inlineStr"/>
+      <c r="FD4" t="inlineStr"/>
+      <c r="FE4" t="inlineStr"/>
+      <c r="FF4" t="inlineStr"/>
+      <c r="FG4" t="inlineStr"/>
+      <c r="FH4" t="inlineStr"/>
+      <c r="FI4" t="inlineStr"/>
+      <c r="FJ4" t="inlineStr"/>
+      <c r="FK4" t="inlineStr"/>
+      <c r="FL4" t="inlineStr"/>
+      <c r="FM4" t="inlineStr"/>
+      <c r="FN4" t="inlineStr"/>
+      <c r="FO4" t="inlineStr"/>
+      <c r="FP4" t="inlineStr"/>
+      <c r="FQ4" t="inlineStr"/>
+      <c r="FR4" t="inlineStr"/>
+      <c r="FS4" t="inlineStr"/>
+      <c r="FT4" t="inlineStr"/>
+      <c r="FU4" t="inlineStr"/>
+      <c r="FV4" t="inlineStr"/>
+      <c r="FW4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.373970091342926</v>
+        <v>18271294300</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3739697933197021</v>
+        <v>18271294300</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3739714026451111</v>
+        <v>21620086600</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3739713430404663</v>
+        <v>21620086600</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3739704191684723</v>
+        <v>21805776300</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3739715814590454</v>
+        <v>21805776300</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3739715814590454</v>
+        <v>21945506200</v>
       </c>
       <c r="H5" t="n">
-        <v>0.3739716410636902</v>
+        <v>21945506200</v>
       </c>
       <c r="I5" t="n">
-        <v>0.373969554901123</v>
+        <v>22073126100</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3739699423313141</v>
+        <v>22073126100</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3739703297615051</v>
+        <v>22176241900</v>
       </c>
       <c r="L5" t="n">
-        <v>0.3739719092845917</v>
+        <v>22176241900</v>
       </c>
       <c r="M5" t="n">
-        <v>0.3739692568778992</v>
+        <v>22283570500</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3739687204360962</v>
+        <v>22283570500</v>
       </c>
       <c r="O5" t="n">
-        <v>0.3739712834358215</v>
+        <v>22384600600</v>
       </c>
       <c r="P5" t="n">
-        <v>0.3739699125289917</v>
+        <v>22384600600</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.3739694952964783</v>
+        <v>22471775500</v>
       </c>
       <c r="R5" t="n">
-        <v>0.373972475528717</v>
+        <v>22471775500</v>
       </c>
       <c r="S5" t="n">
-        <v>0.3739722371101379</v>
+        <v>22532101000</v>
       </c>
       <c r="T5" t="n">
-        <v>0.3739700317382812</v>
+        <v>22532101000</v>
       </c>
       <c r="U5" t="n">
-        <v>0.3739702999591827</v>
+        <v>22616570000</v>
       </c>
       <c r="V5" t="n">
-        <v>0.3739704489707947</v>
+        <v>22616570000</v>
       </c>
       <c r="W5" t="n">
-        <v>0.3739703297615051</v>
+        <v>22706191000</v>
       </c>
       <c r="X5" t="n">
-        <v>0.3739719986915588</v>
+        <v>22706191000</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.3739678859710693</v>
+        <v>22808742600</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.373970627784729</v>
+        <v>22808742600</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3739688396453857</v>
+        <v>22911453900</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.373968243598938</v>
+        <v>22911453900</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.3739708364009857</v>
+        <v>23008489500</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.3739710748195648</v>
+        <v>23008489500</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.3739714622497559</v>
+        <v>23108108300</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.3739728629589081</v>
+        <v>23108108300</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.3739694952964783</v>
+        <v>23200604900</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.3739710450172424</v>
+        <v>23200604900</v>
       </c>
       <c r="AI5" t="n">
-        <v>0.3743055462837219</v>
+        <v>23329446700</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.3739693164825439</v>
+        <v>23329446700</v>
       </c>
       <c r="AK5" t="n">
-        <v>0.3738349080085754</v>
+        <v>23400193500</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.3737640380859375</v>
+        <v>23400193500</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.3738792836666107</v>
+        <v>23504284800</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.3739708960056305</v>
+        <v>23504284800</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.3739576041698456</v>
+        <v>23611049600</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.3736016452312469</v>
+        <v>23611049600</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.3734646439552307</v>
+        <v>23710861600</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.3731843233108521</v>
+        <v>23710861600</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.3730300664901733</v>
+        <v>23831326500</v>
       </c>
       <c r="AT5" t="n">
-        <v>0.3730209469795227</v>
+        <v>23831326500</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.3728436827659607</v>
+        <v>23934081600</v>
       </c>
       <c r="AV5" t="n">
-        <v>0.3728630542755127</v>
+        <v>23934081600</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.3726453185081482</v>
+        <v>24036230300</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.3724945187568665</v>
+        <v>24036230300</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.3723317980766296</v>
+        <v>24128120900</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.371985912322998</v>
+        <v>24128120900</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.3718041777610779</v>
+        <v>24251011300</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.371557205915451</v>
+        <v>24251011300</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.3714287877082825</v>
+        <v>24349983600</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.3713581562042236</v>
+        <v>24349983600</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.3717801570892334</v>
+        <v>24461725000</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.3778453171253204</v>
+        <v>24461725000</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.3853480219841003</v>
+        <v>24559682200</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.3930789232254028</v>
+        <v>24559682200</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.3982595801353455</v>
+        <v>24656367500</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.404346227645874</v>
+        <v>24656367500</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.4118934273719788</v>
+        <v>24756036100</v>
       </c>
       <c r="BL5" t="n">
-        <v>0.4193663895130157</v>
+        <v>24756036100</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.4267885684967041</v>
+        <v>24860263500</v>
       </c>
       <c r="BN5" t="n">
-        <v>0.43413907289505</v>
+        <v>24860263500</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.4416482150554657</v>
+        <v>24961448200</v>
       </c>
       <c r="BP5" t="n">
-        <v>0.4490522146224976</v>
+        <v>24961448200</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.4564083516597748</v>
+        <v>25041257500</v>
       </c>
       <c r="BR5" t="n">
-        <v>0.4638319611549377</v>
+        <v>25041257500</v>
       </c>
       <c r="BS5" t="n">
-        <v>0.4714597761631012</v>
+        <v>25178994100</v>
       </c>
       <c r="BT5" t="n">
-        <v>0.4775876402854919</v>
+        <v>25178994100</v>
       </c>
       <c r="BU5" t="n">
-        <v>0.4849590659141541</v>
+        <v>25324787400</v>
       </c>
       <c r="BV5" t="n">
-        <v>0.4924229681491852</v>
+        <v>25324787400</v>
       </c>
       <c r="BW5" t="n">
-        <v>0.4986508786678314</v>
-      </c>
-      <c r="BX5" t="inlineStr"/>
-      <c r="BY5" t="inlineStr"/>
-      <c r="BZ5" t="inlineStr"/>
-      <c r="CA5" t="inlineStr"/>
-      <c r="CB5" t="inlineStr"/>
-      <c r="CC5" t="inlineStr"/>
-      <c r="CD5" t="inlineStr"/>
-      <c r="CE5" t="inlineStr"/>
-      <c r="CF5" t="inlineStr"/>
-      <c r="CG5" t="inlineStr"/>
-      <c r="CH5" t="inlineStr"/>
-      <c r="CI5" t="inlineStr"/>
-      <c r="CJ5" t="inlineStr"/>
-      <c r="CK5" t="inlineStr"/>
-      <c r="CL5" t="inlineStr"/>
-      <c r="CM5" t="inlineStr"/>
-      <c r="CN5" t="inlineStr"/>
-      <c r="CO5" t="inlineStr"/>
-      <c r="CP5" t="inlineStr"/>
-      <c r="CQ5" t="inlineStr"/>
-      <c r="CR5" t="inlineStr"/>
-      <c r="CS5" t="inlineStr"/>
-      <c r="CT5" t="inlineStr"/>
-      <c r="CU5" t="inlineStr"/>
-      <c r="CV5" t="inlineStr"/>
-      <c r="CW5" t="inlineStr"/>
-      <c r="CX5" t="inlineStr"/>
-      <c r="CY5" t="inlineStr"/>
-      <c r="CZ5" t="inlineStr"/>
-      <c r="DA5" t="inlineStr"/>
-      <c r="DB5" t="inlineStr"/>
-      <c r="DC5" t="inlineStr"/>
-      <c r="DD5" t="inlineStr"/>
-      <c r="DE5" t="inlineStr"/>
-      <c r="DF5" t="inlineStr"/>
-      <c r="DG5" t="inlineStr"/>
-      <c r="DH5" t="inlineStr"/>
-      <c r="DI5" t="inlineStr"/>
-      <c r="DJ5" t="inlineStr"/>
-      <c r="DK5" t="inlineStr"/>
-      <c r="DL5" t="inlineStr"/>
-      <c r="DM5" t="inlineStr"/>
-      <c r="DN5" t="inlineStr"/>
-      <c r="DO5" t="inlineStr"/>
-      <c r="DP5" t="inlineStr"/>
-      <c r="DQ5" t="inlineStr"/>
-      <c r="DR5" t="inlineStr"/>
-      <c r="DS5" t="inlineStr"/>
-      <c r="DT5" t="inlineStr"/>
-      <c r="DU5" t="inlineStr"/>
-      <c r="DV5" t="inlineStr"/>
-      <c r="DW5" t="inlineStr"/>
-      <c r="DX5" t="inlineStr"/>
-      <c r="DY5" t="inlineStr"/>
-      <c r="DZ5" t="inlineStr"/>
-      <c r="EA5" t="inlineStr"/>
-      <c r="EB5" t="inlineStr"/>
-      <c r="EC5" t="inlineStr"/>
-      <c r="ED5" t="inlineStr"/>
-      <c r="EE5" t="inlineStr"/>
-      <c r="EF5" t="inlineStr"/>
-      <c r="EG5" t="inlineStr"/>
-      <c r="EH5" t="inlineStr"/>
-      <c r="EI5" t="inlineStr"/>
-      <c r="EJ5" t="inlineStr"/>
-      <c r="EK5" t="inlineStr"/>
-      <c r="EL5" t="inlineStr"/>
-      <c r="EM5" t="inlineStr"/>
-      <c r="EN5" t="inlineStr"/>
-      <c r="EO5" t="inlineStr"/>
-      <c r="EP5" t="inlineStr"/>
-      <c r="EQ5" t="inlineStr"/>
-      <c r="ER5" t="inlineStr"/>
-      <c r="ES5" t="inlineStr"/>
-      <c r="ET5" t="inlineStr"/>
-      <c r="EU5" t="inlineStr"/>
+        <v>25451565800</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>25451565800</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>25623410600</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>25623410600</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>25804514900</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>25804514900</v>
+      </c>
+      <c r="CC5" t="n">
+        <v>25941073000</v>
+      </c>
+      <c r="CD5" t="n">
+        <v>25941073000</v>
+      </c>
+      <c r="CE5" t="n">
+        <v>26072384700</v>
+      </c>
+      <c r="CF5" t="n">
+        <v>26072384700</v>
+      </c>
+      <c r="CG5" t="n">
+        <v>26203328400</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>26203328400</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>26331189100</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>26331189100</v>
+      </c>
+      <c r="CK5" t="n">
+        <v>26459429100</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>26459429100</v>
+      </c>
+      <c r="CM5" t="n">
+        <v>26576559700</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>26576559700</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>26702170400</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>26702170400</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>26851923500</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>26851923500</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>26975465500</v>
+      </c>
+      <c r="CT5" t="n">
+        <v>26975465500</v>
+      </c>
+      <c r="CU5" t="n">
+        <v>27104332200</v>
+      </c>
+      <c r="CV5" t="n">
+        <v>27104332200</v>
+      </c>
+      <c r="CW5" t="n">
+        <v>27228227500</v>
+      </c>
+      <c r="CX5" t="n">
+        <v>27228227500</v>
+      </c>
+      <c r="CY5" t="n">
+        <v>27354582500</v>
+      </c>
+      <c r="CZ5" t="n">
+        <v>27354582500</v>
+      </c>
+      <c r="DA5" t="n">
+        <v>27474480400</v>
+      </c>
+      <c r="DB5" t="n">
+        <v>27474480400</v>
+      </c>
+      <c r="DC5" t="n">
+        <v>27607612100</v>
+      </c>
+      <c r="DD5" t="n">
+        <v>27607612100</v>
+      </c>
+      <c r="DE5" t="n">
+        <v>27728781300</v>
+      </c>
+      <c r="DF5" t="n">
+        <v>27728781300</v>
+      </c>
+      <c r="DG5" t="n">
+        <v>27881673300</v>
+      </c>
+      <c r="DH5" t="n">
+        <v>27881673300</v>
+      </c>
+      <c r="DI5" t="n">
+        <v>28004511000</v>
+      </c>
+      <c r="DJ5" t="n">
+        <v>28004511000</v>
+      </c>
+      <c r="DK5" t="n">
+        <v>28175800200</v>
+      </c>
+      <c r="DL5" t="n">
+        <v>28175800200</v>
+      </c>
+      <c r="DM5" t="n">
+        <v>28353842400</v>
+      </c>
+      <c r="DN5" t="n">
+        <v>28353842400</v>
+      </c>
+      <c r="DO5" t="n">
+        <v>28503486500</v>
+      </c>
+      <c r="DP5" t="n">
+        <v>28503486500</v>
+      </c>
+      <c r="DQ5" t="n">
+        <v>28627402500</v>
+      </c>
+      <c r="DR5" t="n">
+        <v>28627402500</v>
+      </c>
+      <c r="DS5" t="n">
+        <v>28752547800</v>
+      </c>
+      <c r="DT5" t="n">
+        <v>28752547800</v>
+      </c>
+      <c r="DU5" t="n">
+        <v>28881119000</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>28881119000</v>
+      </c>
+      <c r="DW5" t="n">
+        <v>29010080900</v>
+      </c>
+      <c r="DX5" t="n">
+        <v>29010080900</v>
+      </c>
+      <c r="DY5" t="n">
+        <v>29154536300</v>
+      </c>
+      <c r="DZ5" t="n">
+        <v>29154536300</v>
+      </c>
+      <c r="EA5" t="n">
+        <v>29329233400</v>
+      </c>
+      <c r="EB5" t="n">
+        <v>29329233400</v>
+      </c>
+      <c r="EC5" t="n">
+        <v>29503368100</v>
+      </c>
+      <c r="ED5" t="n">
+        <v>29503368100</v>
+      </c>
+      <c r="EE5" t="n">
+        <v>29656640300</v>
+      </c>
+      <c r="EF5" t="n">
+        <v>29656640300</v>
+      </c>
+      <c r="EG5" t="n">
+        <v>45630498900</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>45630498900</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>45842430500</v>
+      </c>
+      <c r="EJ5" t="n">
+        <v>45842430500</v>
+      </c>
+      <c r="EK5" t="n">
+        <v>46128729500</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>46128729500</v>
+      </c>
+      <c r="EM5" t="n">
+        <v>46404566100</v>
+      </c>
+      <c r="EN5" t="n">
+        <v>46404566100</v>
+      </c>
+      <c r="EO5" t="n">
+        <v>46580296300</v>
+      </c>
+      <c r="EP5" t="n">
+        <v>46580296300</v>
+      </c>
+      <c r="EQ5" t="n">
+        <v>46756213900</v>
+      </c>
+      <c r="ER5" t="n">
+        <v>46756213900</v>
+      </c>
+      <c r="ES5" t="n">
+        <v>46931374000</v>
+      </c>
+      <c r="ET5" t="n">
+        <v>46931374000</v>
+      </c>
+      <c r="EU5" t="n">
+        <v>47104262400</v>
+      </c>
+      <c r="EV5" t="n">
+        <v>47104262400</v>
+      </c>
+      <c r="EW5" t="n">
+        <v>47256300900</v>
+      </c>
+      <c r="EX5" t="n">
+        <v>47256300900</v>
+      </c>
+      <c r="EY5" t="n">
+        <v>47432668500</v>
+      </c>
+      <c r="EZ5" t="n">
+        <v>47432668500</v>
+      </c>
+      <c r="FA5" t="n">
+        <v>47602511500</v>
+      </c>
+      <c r="FB5" t="n">
+        <v>47602511500</v>
+      </c>
+      <c r="FC5" t="n">
+        <v>47722391600</v>
+      </c>
+      <c r="FD5" t="n">
+        <v>47722391600</v>
+      </c>
+      <c r="FE5" t="n">
+        <v>47882529500</v>
+      </c>
+      <c r="FF5" t="n">
+        <v>47882529500</v>
+      </c>
+      <c r="FG5" t="n">
+        <v>48002107100</v>
+      </c>
+      <c r="FH5" t="n">
+        <v>48002107100</v>
+      </c>
+      <c r="FI5" t="n">
+        <v>48133285500</v>
+      </c>
+      <c r="FJ5" t="n">
+        <v>48133285500</v>
+      </c>
+      <c r="FK5" t="n">
+        <v>48258080800</v>
+      </c>
+      <c r="FL5" t="n">
+        <v>48258080800</v>
+      </c>
+      <c r="FM5" t="n">
+        <v>48377417900</v>
+      </c>
+      <c r="FN5" t="n">
+        <v>48377417900</v>
+      </c>
+      <c r="FO5" t="n">
+        <v>48529012700</v>
+      </c>
+      <c r="FP5" t="n">
+        <v>48529012700</v>
+      </c>
+      <c r="FQ5" t="n">
+        <v>48659168900</v>
+      </c>
+      <c r="FR5" t="n">
+        <v>48659168900</v>
+      </c>
+      <c r="FS5" t="n">
+        <v>48782343300</v>
+      </c>
+      <c r="FT5" t="n">
+        <v>48782343300</v>
+      </c>
+      <c r="FU5" t="n">
+        <v>48904176800</v>
+      </c>
+      <c r="FV5" t="n">
+        <v>48904176800</v>
+      </c>
+      <c r="FW5" t="n">
+        <v>60340485000</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>18780165700</v>
+        <v>66</v>
       </c>
       <c r="B6" t="n">
-        <v>18780165700</v>
+        <v>66</v>
       </c>
       <c r="C6" t="n">
-        <v>22052215600</v>
+        <v>66</v>
       </c>
       <c r="D6" t="n">
-        <v>22052215600</v>
+        <v>65</v>
       </c>
       <c r="E6" t="n">
-        <v>22278400900</v>
+        <v>66</v>
       </c>
       <c r="F6" t="n">
-        <v>22278400900</v>
+        <v>65</v>
       </c>
       <c r="G6" t="n">
-        <v>22376785100</v>
+        <v>66</v>
       </c>
       <c r="H6" t="n">
-        <v>22376785100</v>
+        <v>66</v>
       </c>
       <c r="I6" t="n">
-        <v>22493368000</v>
+        <v>66</v>
       </c>
       <c r="J6" t="n">
-        <v>22493368000</v>
+        <v>66</v>
       </c>
       <c r="K6" t="n">
-        <v>22551546900</v>
+        <v>66</v>
       </c>
       <c r="L6" t="n">
-        <v>22551546900</v>
+        <v>66</v>
       </c>
       <c r="M6" t="n">
-        <v>22644035500</v>
+        <v>66</v>
       </c>
       <c r="N6" t="n">
-        <v>22644035500</v>
+        <v>66</v>
       </c>
       <c r="O6" t="n">
-        <v>22735013300</v>
+        <v>66</v>
       </c>
       <c r="P6" t="n">
-        <v>22735013300</v>
+        <v>66</v>
       </c>
       <c r="Q6" t="n">
-        <v>22806519600</v>
+        <v>66</v>
       </c>
       <c r="R6" t="n">
-        <v>22806519600</v>
+        <v>66</v>
       </c>
       <c r="S6" t="n">
-        <v>22895038400</v>
+        <v>65</v>
       </c>
       <c r="T6" t="n">
-        <v>22895038400</v>
+        <v>65</v>
       </c>
       <c r="U6" t="n">
-        <v>22997105400</v>
+        <v>66</v>
       </c>
       <c r="V6" t="n">
-        <v>22997105400</v>
+        <v>66</v>
       </c>
       <c r="W6" t="n">
-        <v>23094706700</v>
+        <v>66</v>
       </c>
       <c r="X6" t="n">
-        <v>23094706700</v>
+        <v>66</v>
       </c>
       <c r="Y6" t="n">
-        <v>23162097700</v>
+        <v>66</v>
       </c>
       <c r="Z6" t="n">
-        <v>23162097700</v>
+        <v>66</v>
       </c>
       <c r="AA6" t="n">
-        <v>23247681000</v>
+        <v>66</v>
       </c>
       <c r="AB6" t="n">
-        <v>23247681000</v>
+        <v>66</v>
       </c>
       <c r="AC6" t="n">
-        <v>23345807100</v>
+        <v>66</v>
       </c>
       <c r="AD6" t="n">
-        <v>23345807100</v>
+        <v>66</v>
       </c>
       <c r="AE6" t="n">
-        <v>23441292900</v>
+        <v>66</v>
       </c>
       <c r="AF6" t="n">
-        <v>23441292900</v>
+        <v>66</v>
       </c>
       <c r="AG6" t="n">
-        <v>23532392300</v>
+        <v>66</v>
       </c>
       <c r="AH6" t="n">
-        <v>23532392300</v>
+        <v>66</v>
       </c>
       <c r="AI6" t="n">
-        <v>23604675100</v>
+        <v>66</v>
       </c>
       <c r="AJ6" t="n">
-        <v>23604675100</v>
+        <v>65</v>
       </c>
       <c r="AK6" t="n">
-        <v>23680124800</v>
+        <v>65</v>
       </c>
       <c r="AL6" t="n">
-        <v>23680124800</v>
+        <v>56</v>
       </c>
       <c r="AM6" t="n">
-        <v>23765098400</v>
+        <v>49</v>
       </c>
       <c r="AN6" t="n">
-        <v>23765098400</v>
+        <v>40</v>
       </c>
       <c r="AO6" t="n">
-        <v>23837413500</v>
+        <v>32</v>
       </c>
       <c r="AP6" t="n">
-        <v>23837413500</v>
+        <v>28</v>
       </c>
       <c r="AQ6" t="n">
-        <v>23917745300</v>
+        <v>19</v>
       </c>
       <c r="AR6" t="n">
-        <v>23917745300</v>
+        <v>12</v>
       </c>
       <c r="AS6" t="n">
-        <v>24020365900</v>
+        <v>3</v>
       </c>
       <c r="AT6" t="n">
-        <v>24020365900</v>
+        <v>2</v>
       </c>
       <c r="AU6" t="n">
-        <v>24118971700</v>
+        <v>-2</v>
       </c>
       <c r="AV6" t="n">
-        <v>24118971700</v>
+        <v>-11</v>
       </c>
       <c r="AW6" t="n">
-        <v>24217720400</v>
+        <v>-16</v>
       </c>
       <c r="AX6" t="n">
-        <v>24217720400</v>
+        <v>-12</v>
       </c>
       <c r="AY6" t="n">
-        <v>24323417900</v>
+        <v>-9</v>
       </c>
       <c r="AZ6" t="n">
-        <v>24323417900</v>
+        <v>-11</v>
       </c>
       <c r="BA6" t="n">
-        <v>24421086800</v>
+        <v>-8</v>
       </c>
       <c r="BB6" t="n">
-        <v>24421086800</v>
+        <v>2</v>
       </c>
       <c r="BC6" t="n">
-        <v>24546944300</v>
+        <v>-9</v>
       </c>
       <c r="BD6" t="n">
-        <v>24546944300</v>
+        <v>3</v>
       </c>
       <c r="BE6" t="n">
-        <v>24645012600</v>
+        <v>1</v>
       </c>
       <c r="BF6" t="n">
-        <v>24645012600</v>
+        <v>-9</v>
       </c>
       <c r="BG6" t="n">
-        <v>24746267400</v>
+        <v>-7</v>
       </c>
       <c r="BH6" t="n">
-        <v>24746267400</v>
+        <v>-12</v>
       </c>
       <c r="BI6" t="n">
-        <v>24872930200</v>
+        <v>-8</v>
       </c>
       <c r="BJ6" t="n">
-        <v>24872930200</v>
+        <v>-7</v>
       </c>
       <c r="BK6" t="n">
-        <v>24996183900</v>
+        <v>-8</v>
       </c>
       <c r="BL6" t="n">
-        <v>24996183900</v>
+        <v>-5</v>
       </c>
       <c r="BM6" t="n">
-        <v>25080462200</v>
+        <v>-9</v>
       </c>
       <c r="BN6" t="n">
-        <v>25080462200</v>
+        <v>-10</v>
       </c>
       <c r="BO6" t="n">
-        <v>25194818800</v>
+        <v>-15</v>
       </c>
       <c r="BP6" t="n">
-        <v>25194818800</v>
+        <v>-13</v>
       </c>
       <c r="BQ6" t="n">
-        <v>25312267600</v>
+        <v>53</v>
       </c>
       <c r="BR6" t="n">
-        <v>25312267600</v>
+        <v>52</v>
       </c>
       <c r="BS6" t="n">
-        <v>25442147800</v>
+        <v>54</v>
       </c>
       <c r="BT6" t="n">
-        <v>25442147800</v>
+        <v>44</v>
       </c>
       <c r="BU6" t="n">
-        <v>25554796400</v>
+        <v>34</v>
       </c>
       <c r="BV6" t="n">
-        <v>25554796400</v>
+        <v>25</v>
       </c>
       <c r="BW6" t="n">
-        <v>25668586900</v>
+        <v>13</v>
       </c>
       <c r="BX6" t="n">
-        <v>25668586900</v>
+        <v>3</v>
       </c>
       <c r="BY6" t="n">
-        <v>25810858000</v>
+        <v>1</v>
       </c>
       <c r="BZ6" t="n">
-        <v>25810858000</v>
+        <v>-11</v>
       </c>
       <c r="CA6" t="n">
-        <v>25916133400</v>
+        <v>-9</v>
       </c>
       <c r="CB6" t="n">
-        <v>25916133400</v>
+        <v>-10</v>
       </c>
       <c r="CC6" t="n">
-        <v>26044915400</v>
+        <v>-6</v>
       </c>
       <c r="CD6" t="n">
-        <v>26044915400</v>
+        <v>-6</v>
       </c>
       <c r="CE6" t="n">
-        <v>26115482100</v>
+        <v>-12</v>
       </c>
       <c r="CF6" t="n">
-        <v>26115482100</v>
+        <v>-9</v>
       </c>
       <c r="CG6" t="n">
-        <v>26180892700</v>
+        <v>-10</v>
       </c>
       <c r="CH6" t="n">
-        <v>26180892700</v>
+        <v>-9</v>
       </c>
       <c r="CI6" t="n">
-        <v>26264166300</v>
+        <v>-10</v>
       </c>
       <c r="CJ6" t="n">
-        <v>26264166300</v>
+        <v>-6</v>
       </c>
       <c r="CK6" t="n">
-        <v>26337855900</v>
-      </c>
-      <c r="CL6" t="n">
-        <v>26337855900</v>
-      </c>
-      <c r="CM6" t="n">
-        <v>26465425200</v>
-      </c>
-      <c r="CN6" t="n">
-        <v>26465425200</v>
-      </c>
-      <c r="CO6" t="n">
-        <v>26588645000</v>
-      </c>
-      <c r="CP6" t="n">
-        <v>26588645000</v>
-      </c>
-      <c r="CQ6" t="n">
-        <v>26713477600</v>
-      </c>
-      <c r="CR6" t="n">
-        <v>26713477600</v>
-      </c>
-      <c r="CS6" t="n">
-        <v>26787731000</v>
-      </c>
-      <c r="CT6" t="n">
-        <v>26787731000</v>
-      </c>
-      <c r="CU6" t="n">
-        <v>26861142900</v>
-      </c>
-      <c r="CV6" t="n">
-        <v>26861142900</v>
-      </c>
-      <c r="CW6" t="n">
-        <v>26936224400</v>
-      </c>
-      <c r="CX6" t="n">
-        <v>26936224400</v>
-      </c>
-      <c r="CY6" t="n">
-        <v>27041674700</v>
-      </c>
-      <c r="CZ6" t="n">
-        <v>27041674700</v>
-      </c>
-      <c r="DA6" t="n">
-        <v>27166024600</v>
-      </c>
-      <c r="DB6" t="n">
-        <v>27166024600</v>
-      </c>
-      <c r="DC6" t="n">
-        <v>27234096700</v>
-      </c>
-      <c r="DD6" t="n">
-        <v>27234096700</v>
-      </c>
-      <c r="DE6" t="n">
-        <v>27309536200</v>
-      </c>
-      <c r="DF6" t="n">
-        <v>27309536200</v>
-      </c>
-      <c r="DG6" t="n">
-        <v>27381775300</v>
-      </c>
-      <c r="DH6" t="n">
-        <v>27381775300</v>
-      </c>
-      <c r="DI6" t="n">
-        <v>27462053900</v>
-      </c>
-      <c r="DJ6" t="n">
-        <v>27462053900</v>
-      </c>
-      <c r="DK6" t="n">
-        <v>27567886400</v>
-      </c>
-      <c r="DL6" t="n">
-        <v>27567886400</v>
-      </c>
-      <c r="DM6" t="n">
-        <v>27717555800</v>
-      </c>
-      <c r="DN6" t="n">
-        <v>27717555800</v>
-      </c>
-      <c r="DO6" t="n">
-        <v>27866761300</v>
-      </c>
-      <c r="DP6" t="n">
-        <v>27866761300</v>
-      </c>
-      <c r="DQ6" t="n">
-        <v>28009068100</v>
-      </c>
-      <c r="DR6" t="n">
-        <v>28009068100</v>
-      </c>
-      <c r="DS6" t="n">
-        <v>28085059600</v>
-      </c>
-      <c r="DT6" t="n">
-        <v>28085059600</v>
-      </c>
-      <c r="DU6" t="n">
-        <v>28241065800</v>
-      </c>
-      <c r="DV6" t="n">
-        <v>28241065800</v>
-      </c>
-      <c r="DW6" t="n">
-        <v>28393781000</v>
-      </c>
-      <c r="DX6" t="n">
-        <v>28393781000</v>
-      </c>
-      <c r="DY6" t="n">
-        <v>28540664100</v>
-      </c>
-      <c r="DZ6" t="n">
-        <v>28540664100</v>
-      </c>
-      <c r="EA6" t="n">
-        <v>28692842200</v>
-      </c>
-      <c r="EB6" t="n">
-        <v>28692842200</v>
-      </c>
-      <c r="EC6" t="n">
-        <v>28842540700</v>
-      </c>
-      <c r="ED6" t="n">
-        <v>28842540700</v>
-      </c>
-      <c r="EE6" t="n">
-        <v>28985980100</v>
-      </c>
-      <c r="EF6" t="n">
-        <v>28985980100</v>
-      </c>
-      <c r="EG6" t="n">
-        <v>29145233200</v>
-      </c>
-      <c r="EH6" t="n">
-        <v>29145233200</v>
-      </c>
-      <c r="EI6" t="n">
-        <v>29291400700</v>
-      </c>
-      <c r="EJ6" t="n">
-        <v>29291400700</v>
-      </c>
-      <c r="EK6" t="n">
-        <v>29445217400</v>
-      </c>
-      <c r="EL6" t="n">
-        <v>29445217400</v>
-      </c>
-      <c r="EM6" t="n">
-        <v>29592607900</v>
-      </c>
-      <c r="EN6" t="n">
-        <v>29592607900</v>
-      </c>
-      <c r="EO6" t="n">
-        <v>29715489500</v>
-      </c>
-      <c r="EP6" t="n">
-        <v>29715489500</v>
-      </c>
-      <c r="EQ6" t="n">
-        <v>29866018900</v>
-      </c>
-      <c r="ER6" t="n">
-        <v>29866018900</v>
-      </c>
-      <c r="ES6" t="n">
-        <v>30015984900</v>
-      </c>
-      <c r="ET6" t="n">
-        <v>30015984900</v>
-      </c>
-      <c r="EU6" t="n">
-        <v>68799082000</v>
-      </c>
+        <v>-7</v>
+      </c>
+      <c r="CL6" t="inlineStr"/>
+      <c r="CM6" t="inlineStr"/>
+      <c r="CN6" t="inlineStr"/>
+      <c r="CO6" t="inlineStr"/>
+      <c r="CP6" t="inlineStr"/>
+      <c r="CQ6" t="inlineStr"/>
+      <c r="CR6" t="inlineStr"/>
+      <c r="CS6" t="inlineStr"/>
+      <c r="CT6" t="inlineStr"/>
+      <c r="CU6" t="inlineStr"/>
+      <c r="CV6" t="inlineStr"/>
+      <c r="CW6" t="inlineStr"/>
+      <c r="CX6" t="inlineStr"/>
+      <c r="CY6" t="inlineStr"/>
+      <c r="CZ6" t="inlineStr"/>
+      <c r="DA6" t="inlineStr"/>
+      <c r="DB6" t="inlineStr"/>
+      <c r="DC6" t="inlineStr"/>
+      <c r="DD6" t="inlineStr"/>
+      <c r="DE6" t="inlineStr"/>
+      <c r="DF6" t="inlineStr"/>
+      <c r="DG6" t="inlineStr"/>
+      <c r="DH6" t="inlineStr"/>
+      <c r="DI6" t="inlineStr"/>
+      <c r="DJ6" t="inlineStr"/>
+      <c r="DK6" t="inlineStr"/>
+      <c r="DL6" t="inlineStr"/>
+      <c r="DM6" t="inlineStr"/>
+      <c r="DN6" t="inlineStr"/>
+      <c r="DO6" t="inlineStr"/>
+      <c r="DP6" t="inlineStr"/>
+      <c r="DQ6" t="inlineStr"/>
+      <c r="DR6" t="inlineStr"/>
+      <c r="DS6" t="inlineStr"/>
+      <c r="DT6" t="inlineStr"/>
+      <c r="DU6" t="inlineStr"/>
+      <c r="DV6" t="inlineStr"/>
+      <c r="DW6" t="inlineStr"/>
+      <c r="DX6" t="inlineStr"/>
+      <c r="DY6" t="inlineStr"/>
+      <c r="DZ6" t="inlineStr"/>
+      <c r="EA6" t="inlineStr"/>
+      <c r="EB6" t="inlineStr"/>
+      <c r="EC6" t="inlineStr"/>
+      <c r="ED6" t="inlineStr"/>
+      <c r="EE6" t="inlineStr"/>
+      <c r="EF6" t="inlineStr"/>
+      <c r="EG6" t="inlineStr"/>
+      <c r="EH6" t="inlineStr"/>
+      <c r="EI6" t="inlineStr"/>
+      <c r="EJ6" t="inlineStr"/>
+      <c r="EK6" t="inlineStr"/>
+      <c r="EL6" t="inlineStr"/>
+      <c r="EM6" t="inlineStr"/>
+      <c r="EN6" t="inlineStr"/>
+      <c r="EO6" t="inlineStr"/>
+      <c r="EP6" t="inlineStr"/>
+      <c r="EQ6" t="inlineStr"/>
+      <c r="ER6" t="inlineStr"/>
+      <c r="ES6" t="inlineStr"/>
+      <c r="ET6" t="inlineStr"/>
+      <c r="EU6" t="inlineStr"/>
+      <c r="EV6" t="inlineStr"/>
+      <c r="EW6" t="inlineStr"/>
+      <c r="EX6" t="inlineStr"/>
+      <c r="EY6" t="inlineStr"/>
+      <c r="EZ6" t="inlineStr"/>
+      <c r="FA6" t="inlineStr"/>
+      <c r="FB6" t="inlineStr"/>
+      <c r="FC6" t="inlineStr"/>
+      <c r="FD6" t="inlineStr"/>
+      <c r="FE6" t="inlineStr"/>
+      <c r="FF6" t="inlineStr"/>
+      <c r="FG6" t="inlineStr"/>
+      <c r="FH6" t="inlineStr"/>
+      <c r="FI6" t="inlineStr"/>
+      <c r="FJ6" t="inlineStr"/>
+      <c r="FK6" t="inlineStr"/>
+      <c r="FL6" t="inlineStr"/>
+      <c r="FM6" t="inlineStr"/>
+      <c r="FN6" t="inlineStr"/>
+      <c r="FO6" t="inlineStr"/>
+      <c r="FP6" t="inlineStr"/>
+      <c r="FQ6" t="inlineStr"/>
+      <c r="FR6" t="inlineStr"/>
+      <c r="FS6" t="inlineStr"/>
+      <c r="FT6" t="inlineStr"/>
+      <c r="FU6" t="inlineStr"/>
+      <c r="FV6" t="inlineStr"/>
+      <c r="FW6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-123</v>
+        <v>-0.06705316156148911</v>
       </c>
       <c r="B7" t="n">
-        <v>-124</v>
+        <v>-0.06705673784017563</v>
       </c>
       <c r="C7" t="n">
-        <v>-124</v>
+        <v>-0.06705763190984726</v>
       </c>
       <c r="D7" t="n">
-        <v>-124</v>
+        <v>-0.06705210357904434</v>
       </c>
       <c r="E7" t="n">
-        <v>-124</v>
+        <v>-0.06706196814775467</v>
       </c>
       <c r="F7" t="n">
-        <v>-124</v>
+        <v>-0.06705477088689804</v>
       </c>
       <c r="G7" t="n">
-        <v>-124</v>
+        <v>-0.06705644726753235</v>
       </c>
       <c r="H7" t="n">
-        <v>-124</v>
+        <v>-0.06705763190984726</v>
       </c>
       <c r="I7" t="n">
-        <v>-125</v>
+        <v>-0.06705751270055771</v>
       </c>
       <c r="J7" t="n">
-        <v>-124</v>
+        <v>-0.067055843770504</v>
       </c>
       <c r="K7" t="n">
-        <v>-124</v>
+        <v>-0.06705840677022934</v>
       </c>
       <c r="L7" t="n">
-        <v>-124</v>
+        <v>-0.06705673784017563</v>
       </c>
       <c r="M7" t="n">
-        <v>-124</v>
+        <v>-0.06705751270055771</v>
       </c>
       <c r="N7" t="n">
-        <v>-124</v>
+        <v>-0.06705734133720398</v>
       </c>
       <c r="O7" t="n">
-        <v>-125</v>
+        <v>-0.06705940514802933</v>
       </c>
       <c r="P7" t="n">
-        <v>-123</v>
+        <v>-0.067055843770504</v>
       </c>
       <c r="Q7" t="n">
-        <v>-123</v>
+        <v>-0.06706119328737259</v>
       </c>
       <c r="R7" t="n">
-        <v>-124</v>
+        <v>-0.06705852597951889</v>
       </c>
       <c r="S7" t="n">
-        <v>-124</v>
+        <v>-0.06705316156148911</v>
       </c>
       <c r="T7" t="n">
-        <v>-124</v>
+        <v>-0.0670628622174263</v>
       </c>
       <c r="U7" t="n">
-        <v>-123</v>
+        <v>-0.06705930829048157</v>
       </c>
       <c r="V7" t="n">
-        <v>-124</v>
+        <v>-0.067055843770504</v>
       </c>
       <c r="W7" t="n">
-        <v>-124</v>
+        <v>-0.06705762445926666</v>
       </c>
       <c r="X7" t="n">
-        <v>-124</v>
+        <v>-0.06705406308174133</v>
       </c>
       <c r="Y7" t="n">
-        <v>-124</v>
+        <v>-0.06705763190984726</v>
       </c>
       <c r="Z7" t="n">
-        <v>-123</v>
+        <v>-0.06705138087272644</v>
       </c>
       <c r="AA7" t="n">
-        <v>-124</v>
+        <v>-0.06705751270055771</v>
       </c>
       <c r="AB7" t="n">
-        <v>-124</v>
+        <v>-0.0670628696680069</v>
       </c>
       <c r="AC7" t="n">
-        <v>-124</v>
+        <v>-0.06705673784017563</v>
       </c>
       <c r="AD7" t="n">
-        <v>-124</v>
+        <v>-0.06705940514802933</v>
       </c>
       <c r="AE7" t="n">
-        <v>-124</v>
+        <v>-0.06705672293901443</v>
       </c>
       <c r="AF7" t="n">
-        <v>-124</v>
+        <v>-0.06705644726753235</v>
       </c>
       <c r="AG7" t="n">
-        <v>-124</v>
+        <v>-0.06706126034259796</v>
       </c>
       <c r="AH7" t="n">
-        <v>-123</v>
+        <v>-0.06705940514802933</v>
       </c>
       <c r="AI7" t="n">
-        <v>-125</v>
+        <v>-0.06705940514802933</v>
       </c>
       <c r="AJ7" t="n">
-        <v>-121</v>
+        <v>-0.06705719977617264</v>
       </c>
       <c r="AK7" t="n">
-        <v>-110</v>
+        <v>-0.06845846772193909</v>
       </c>
       <c r="AL7" t="n">
-        <v>-108</v>
+        <v>-0.07153720408678055</v>
       </c>
       <c r="AM7" t="n">
-        <v>-91</v>
+        <v>-0.07532136142253876</v>
       </c>
       <c r="AN7" t="n">
-        <v>-88</v>
+        <v>-0.07895633578300476</v>
       </c>
       <c r="AO7" t="n">
-        <v>-77</v>
+        <v>-0.08186151087284088</v>
       </c>
       <c r="AP7" t="n">
-        <v>-73</v>
+        <v>-0.08357339352369308</v>
       </c>
       <c r="AQ7" t="n">
-        <v>-65</v>
+        <v>-0.08611632883548737</v>
       </c>
       <c r="AR7" t="n">
-        <v>-59</v>
+        <v>-0.0882035493850708</v>
       </c>
       <c r="AS7" t="n">
-        <v>-55</v>
+        <v>-0.0898192897439003</v>
       </c>
       <c r="AT7" t="n">
-        <v>-42</v>
+        <v>-0.09048603475093842</v>
       </c>
       <c r="AU7" t="n">
-        <v>-37</v>
+        <v>-0.09143159538507462</v>
       </c>
       <c r="AV7" t="n">
-        <v>-26</v>
+        <v>-0.09177464246749878</v>
       </c>
       <c r="AW7" t="n">
-        <v>-21</v>
+        <v>-0.0921793133020401</v>
       </c>
       <c r="AX7" t="n">
-        <v>-13</v>
+        <v>-0.09215624630451202</v>
       </c>
       <c r="AY7" t="n">
-        <v>-11</v>
+        <v>-0.09224453568458557</v>
       </c>
       <c r="AZ7" t="n">
-        <v>-3</v>
+        <v>-0.09206276386976242</v>
       </c>
       <c r="BA7" t="n">
-        <v>0</v>
+        <v>-0.09176106750965118</v>
       </c>
       <c r="BB7" t="n">
-        <v>1</v>
+        <v>-0.09153667092323303</v>
       </c>
       <c r="BC7" t="n">
-        <v>2</v>
+        <v>-0.09092005342245102</v>
       </c>
       <c r="BD7" t="n">
-        <v>4</v>
+        <v>-0.09127230197191238</v>
       </c>
       <c r="BE7" t="n">
-        <v>6</v>
+        <v>-0.0916549414396286</v>
       </c>
       <c r="BF7" t="n">
-        <v>6</v>
+        <v>-0.09196589887142181</v>
       </c>
       <c r="BG7" t="n">
-        <v>8</v>
+        <v>-0.09298316389322281</v>
       </c>
       <c r="BH7" t="n">
-        <v>10</v>
+        <v>-0.09282274544239044</v>
       </c>
       <c r="BI7" t="n">
-        <v>10</v>
+        <v>-0.09249222278594971</v>
       </c>
       <c r="BJ7" t="n">
-        <v>10</v>
+        <v>-0.0931212529540062</v>
       </c>
       <c r="BK7" t="n">
-        <v>3</v>
+        <v>-0.09289023280143738</v>
       </c>
       <c r="BL7" t="n">
-        <v>-2</v>
+        <v>-0.09240705519914627</v>
       </c>
       <c r="BM7" t="n">
-        <v>-4</v>
+        <v>-0.09269608557224274</v>
       </c>
       <c r="BN7" t="n">
-        <v>-4</v>
+        <v>-0.09292198717594147</v>
       </c>
       <c r="BO7" t="n">
-        <v>1</v>
+        <v>-0.09257658571004868</v>
       </c>
       <c r="BP7" t="n">
-        <v>3</v>
+        <v>-0.09183460474014282</v>
       </c>
       <c r="BQ7" t="n">
-        <v>7</v>
+        <v>-0.06708595901727676</v>
       </c>
       <c r="BR7" t="n">
-        <v>4</v>
+        <v>-0.06849204003810883</v>
       </c>
       <c r="BS7" t="n">
-        <v>3</v>
+        <v>-0.07458639889955521</v>
       </c>
       <c r="BT7" t="n">
-        <v>8</v>
+        <v>-0.07793766260147095</v>
       </c>
       <c r="BU7" t="n">
-        <v>0</v>
+        <v>-0.08191720396280289</v>
       </c>
       <c r="BV7" t="n">
-        <v>2</v>
+        <v>-0.08567574620246887</v>
       </c>
       <c r="BW7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX7" t="inlineStr"/>
-      <c r="BY7" t="inlineStr"/>
-      <c r="BZ7" t="inlineStr"/>
-      <c r="CA7" t="inlineStr"/>
-      <c r="CB7" t="inlineStr"/>
-      <c r="CC7" t="inlineStr"/>
-      <c r="CD7" t="inlineStr"/>
-      <c r="CE7" t="inlineStr"/>
-      <c r="CF7" t="inlineStr"/>
-      <c r="CG7" t="inlineStr"/>
-      <c r="CH7" t="inlineStr"/>
-      <c r="CI7" t="inlineStr"/>
-      <c r="CJ7" t="inlineStr"/>
-      <c r="CK7" t="inlineStr"/>
+        <v>-0.08886031806468964</v>
+      </c>
+      <c r="BX7" t="n">
+        <v>-0.09037581831216812</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>-0.09246043115854263</v>
+      </c>
+      <c r="BZ7" t="n">
+        <v>-0.09236221015453339</v>
+      </c>
+      <c r="CA7" t="n">
+        <v>-0.09247145056724548</v>
+      </c>
+      <c r="CB7" t="n">
+        <v>-0.0925169363617897</v>
+      </c>
+      <c r="CC7" t="n">
+        <v>-0.09319400042295456</v>
+      </c>
+      <c r="CD7" t="n">
+        <v>-0.09349717199802399</v>
+      </c>
+      <c r="CE7" t="n">
+        <v>-0.09330660849809647</v>
+      </c>
+      <c r="CF7" t="n">
+        <v>-0.0938132256269455</v>
+      </c>
+      <c r="CG7" t="n">
+        <v>-0.09317471086978912</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>-0.09258635342121124</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>-0.09218883514404297</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>-0.0921570211648941</v>
+      </c>
+      <c r="CK7" t="n">
+        <v>-0.09155506640672684</v>
+      </c>
       <c r="CL7" t="inlineStr"/>
       <c r="CM7" t="inlineStr"/>
       <c r="CN7" t="inlineStr"/>
@@ -2857,6 +3277,34 @@
       <c r="ES7" t="inlineStr"/>
       <c r="ET7" t="inlineStr"/>
       <c r="EU7" t="inlineStr"/>
+      <c r="EV7" t="inlineStr"/>
+      <c r="EW7" t="inlineStr"/>
+      <c r="EX7" t="inlineStr"/>
+      <c r="EY7" t="inlineStr"/>
+      <c r="EZ7" t="inlineStr"/>
+      <c r="FA7" t="inlineStr"/>
+      <c r="FB7" t="inlineStr"/>
+      <c r="FC7" t="inlineStr"/>
+      <c r="FD7" t="inlineStr"/>
+      <c r="FE7" t="inlineStr"/>
+      <c r="FF7" t="inlineStr"/>
+      <c r="FG7" t="inlineStr"/>
+      <c r="FH7" t="inlineStr"/>
+      <c r="FI7" t="inlineStr"/>
+      <c r="FJ7" t="inlineStr"/>
+      <c r="FK7" t="inlineStr"/>
+      <c r="FL7" t="inlineStr"/>
+      <c r="FM7" t="inlineStr"/>
+      <c r="FN7" t="inlineStr"/>
+      <c r="FO7" t="inlineStr"/>
+      <c r="FP7" t="inlineStr"/>
+      <c r="FQ7" t="inlineStr"/>
+      <c r="FR7" t="inlineStr"/>
+      <c r="FS7" t="inlineStr"/>
+      <c r="FT7" t="inlineStr"/>
+      <c r="FU7" t="inlineStr"/>
+      <c r="FV7" t="inlineStr"/>
+      <c r="FW7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>